<commit_message>
updated feature selection file
</commit_message>
<xml_diff>
--- a/hackerearth_ml3_adclick/analysis_graphs/feature_selection.xlsx
+++ b/hackerearth_ml3_adclick/analysis_graphs/feature_selection.xlsx
@@ -1,18 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18229"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dragon\Documents\PythonProjects\Kaggle\hackerearth_ml3_adclick\analysis_graphs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vaibhav.ojha\Desktop\PythonProjects\Kaggle\hackerearth_ml3_adclick\analysis_graphs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1872" yWindow="0" windowWidth="22104" windowHeight="11016"/>
+    <workbookView xWindow="3648" yWindow="0" windowWidth="22104" windowHeight="11016" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="76">
   <si>
     <t>chi square values</t>
   </si>
@@ -138,6 +139,120 @@
   </si>
   <si>
     <t>devid_3</t>
+  </si>
+  <si>
+    <t>countrycode_0</t>
+  </si>
+  <si>
+    <t>countrycode_1</t>
+  </si>
+  <si>
+    <t>countrycode_2</t>
+  </si>
+  <si>
+    <t>countrycode_3</t>
+  </si>
+  <si>
+    <t>countrycode_4</t>
+  </si>
+  <si>
+    <t>countrycode_5</t>
+  </si>
+  <si>
+    <t>browserid_0</t>
+  </si>
+  <si>
+    <t>datetime_day_0</t>
+  </si>
+  <si>
+    <t>datetime_day_1</t>
+  </si>
+  <si>
+    <t>datetime_day_5</t>
+  </si>
+  <si>
+    <t>datetime_day_3</t>
+  </si>
+  <si>
+    <t>datetime_day_6</t>
+  </si>
+  <si>
+    <t>datetime_day_2</t>
+  </si>
+  <si>
+    <t>datetime_day_4</t>
+  </si>
+  <si>
+    <t>datetime_hour_0</t>
+  </si>
+  <si>
+    <t>datetime_hour_1</t>
+  </si>
+  <si>
+    <t>datetime_hour_4</t>
+  </si>
+  <si>
+    <t>datetime_hour_3</t>
+  </si>
+  <si>
+    <t>datetime_hour_6</t>
+  </si>
+  <si>
+    <t>datetime_hour_2</t>
+  </si>
+  <si>
+    <t>datetime_hour_5</t>
+  </si>
+  <si>
+    <t>datetime_hour_7</t>
+  </si>
+  <si>
+    <t>datetime_hour_8</t>
+  </si>
+  <si>
+    <t>datetime_hour_9</t>
+  </si>
+  <si>
+    <t>datetime_hour_10</t>
+  </si>
+  <si>
+    <t>datetime_hour_11</t>
+  </si>
+  <si>
+    <t>datetime_hour_12</t>
+  </si>
+  <si>
+    <t>datetime_hour_13</t>
+  </si>
+  <si>
+    <t>datetime_hour_14</t>
+  </si>
+  <si>
+    <t>datetime_hour_15</t>
+  </si>
+  <si>
+    <t>datetime_hour_16</t>
+  </si>
+  <si>
+    <t>datetime_hour_17</t>
+  </si>
+  <si>
+    <t>datetime_hour_18</t>
+  </si>
+  <si>
+    <t>datetime_hour_19</t>
+  </si>
+  <si>
+    <t>datetime_hour_20</t>
+  </si>
+  <si>
+    <t>datetime_hour_21</t>
+  </si>
+  <si>
+    <t>datetime_hour_22</t>
+  </si>
+  <si>
+    <t>datetime_hour_23</t>
   </si>
 </sst>
 </file>
@@ -146,7 +261,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="171" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -194,64 +309,14 @@
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="7">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -584,8 +649,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1777,4 +1842,982 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I53"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L12" sqref="L12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="16.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="2">
+        <v>355138.342</v>
+      </c>
+      <c r="D3" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3" s="1">
+        <v>1.7337573200000001E-5</v>
+      </c>
+      <c r="H3" t="s">
+        <v>10</v>
+      </c>
+      <c r="I3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="2">
+        <v>429213.31599999999</v>
+      </c>
+      <c r="D4" s="1">
+        <v>0</v>
+      </c>
+      <c r="E4" s="1">
+        <v>9.2234408799999997E-6</v>
+      </c>
+      <c r="H4">
+        <v>0.1</v>
+      </c>
+      <c r="I4">
+        <v>2.71</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="2">
+        <v>367088.40100000001</v>
+      </c>
+      <c r="D5" s="1">
+        <v>0</v>
+      </c>
+      <c r="E5" s="1">
+        <v>2.06433299E-4</v>
+      </c>
+      <c r="H5">
+        <v>0.05</v>
+      </c>
+      <c r="I5">
+        <v>3.84</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>3</v>
+      </c>
+      <c r="B6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="2">
+        <v>7230137.4000000004</v>
+      </c>
+      <c r="D6" s="1">
+        <v>0</v>
+      </c>
+      <c r="E6" s="1">
+        <v>1.51952052E-5</v>
+      </c>
+      <c r="H6">
+        <v>0.01</v>
+      </c>
+      <c r="I6">
+        <v>6.63</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>4</v>
+      </c>
+      <c r="B7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C7" s="2">
+        <v>1433877.96</v>
+      </c>
+      <c r="D7" s="1">
+        <v>0</v>
+      </c>
+      <c r="E7" s="1">
+        <v>5.1081965E-2</v>
+      </c>
+      <c r="H7">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="I7">
+        <v>7.88</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>5</v>
+      </c>
+      <c r="B8" t="s">
+        <v>39</v>
+      </c>
+      <c r="C8" s="2">
+        <v>3402912.46</v>
+      </c>
+      <c r="D8" s="1">
+        <v>0</v>
+      </c>
+      <c r="E8" s="1">
+        <v>0.105516158</v>
+      </c>
+      <c r="H8">
+        <v>1E-3</v>
+      </c>
+      <c r="I8">
+        <v>10.83</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>6</v>
+      </c>
+      <c r="B9" t="s">
+        <v>40</v>
+      </c>
+      <c r="C9" s="2">
+        <v>3922735.81</v>
+      </c>
+      <c r="D9" s="1">
+        <v>0</v>
+      </c>
+      <c r="E9" s="1">
+        <v>0.24401761</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>7</v>
+      </c>
+      <c r="B10" t="s">
+        <v>41</v>
+      </c>
+      <c r="C10" s="2">
+        <v>1882656.23</v>
+      </c>
+      <c r="D10" s="1">
+        <v>0</v>
+      </c>
+      <c r="E10" s="1">
+        <v>0.102639786</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>8</v>
+      </c>
+      <c r="B11" t="s">
+        <v>42</v>
+      </c>
+      <c r="C11" s="2">
+        <v>182854.152</v>
+      </c>
+      <c r="D11" s="1">
+        <v>0</v>
+      </c>
+      <c r="E11" s="1">
+        <v>1.59798458E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>9</v>
+      </c>
+      <c r="B12" t="s">
+        <v>43</v>
+      </c>
+      <c r="C12" s="2">
+        <v>184865.79199999999</v>
+      </c>
+      <c r="D12" s="1">
+        <v>0</v>
+      </c>
+      <c r="E12" s="1">
+        <v>1.5661713000000001E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>10</v>
+      </c>
+      <c r="B13" t="s">
+        <v>44</v>
+      </c>
+      <c r="C13" s="2">
+        <v>549.83858599999996</v>
+      </c>
+      <c r="D13" s="1">
+        <v>1.36491092E-121</v>
+      </c>
+      <c r="E13" s="1">
+        <v>3.9819249200000002E-3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>11</v>
+      </c>
+      <c r="B14" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" s="2">
+        <v>1965759.67</v>
+      </c>
+      <c r="D14" s="1">
+        <v>0</v>
+      </c>
+      <c r="E14" s="1">
+        <v>8.6760738000000004E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>12</v>
+      </c>
+      <c r="B15" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15" s="2">
+        <v>2995640.15</v>
+      </c>
+      <c r="D15" s="1">
+        <v>0</v>
+      </c>
+      <c r="E15" s="1">
+        <v>0.123231378</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>13</v>
+      </c>
+      <c r="B16" t="s">
+        <v>30</v>
+      </c>
+      <c r="C16" s="2">
+        <v>139916.91099999999</v>
+      </c>
+      <c r="D16" s="1">
+        <v>0</v>
+      </c>
+      <c r="E16" s="1">
+        <v>5.0439913699999998E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>14</v>
+      </c>
+      <c r="B17" t="s">
+        <v>31</v>
+      </c>
+      <c r="C17" s="2">
+        <v>53.453002599999998</v>
+      </c>
+      <c r="D17" s="1">
+        <v>2.6485375000000002E-13</v>
+      </c>
+      <c r="E17" s="1">
+        <v>6.3685785099999997E-4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>15</v>
+      </c>
+      <c r="B18" t="s">
+        <v>32</v>
+      </c>
+      <c r="C18" s="2">
+        <v>55.359001300000003</v>
+      </c>
+      <c r="D18" s="1">
+        <v>1.00409018E-13</v>
+      </c>
+      <c r="E18" s="1">
+        <v>2.9022666399999999E-4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>16</v>
+      </c>
+      <c r="B19" t="s">
+        <v>34</v>
+      </c>
+      <c r="C19" s="2">
+        <v>90.685528700000006</v>
+      </c>
+      <c r="D19" s="1">
+        <v>1.68420542E-21</v>
+      </c>
+      <c r="E19" s="1">
+        <v>1.17057789E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>17</v>
+      </c>
+      <c r="B20" t="s">
+        <v>35</v>
+      </c>
+      <c r="C20" s="2">
+        <v>728024.82400000002</v>
+      </c>
+      <c r="D20" s="1">
+        <v>0</v>
+      </c>
+      <c r="E20" s="1">
+        <v>7.1191111700000004E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>18</v>
+      </c>
+      <c r="B21" t="s">
+        <v>36</v>
+      </c>
+      <c r="C21" s="2">
+        <v>16895.480299999999</v>
+      </c>
+      <c r="D21" s="1">
+        <v>0</v>
+      </c>
+      <c r="E21" s="1">
+        <v>2.0059922000000001E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>19</v>
+      </c>
+      <c r="B22" t="s">
+        <v>37</v>
+      </c>
+      <c r="C22" s="2">
+        <v>1955934.32</v>
+      </c>
+      <c r="D22" s="1">
+        <v>0</v>
+      </c>
+      <c r="E22" s="1">
+        <v>5.9929367800000001E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>20</v>
+      </c>
+      <c r="B23" t="s">
+        <v>45</v>
+      </c>
+      <c r="C23" s="2">
+        <v>2939.2909100000002</v>
+      </c>
+      <c r="D23" s="1">
+        <v>0</v>
+      </c>
+      <c r="E23" s="1">
+        <v>5.3523122100000004E-4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>21</v>
+      </c>
+      <c r="B24" t="s">
+        <v>46</v>
+      </c>
+      <c r="C24" s="2">
+        <v>2526.0420600000002</v>
+      </c>
+      <c r="D24" s="1">
+        <v>0</v>
+      </c>
+      <c r="E24" s="1">
+        <v>1.88174024E-4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>22</v>
+      </c>
+      <c r="B25" t="s">
+        <v>50</v>
+      </c>
+      <c r="C25" s="2">
+        <v>102.108862</v>
+      </c>
+      <c r="D25" s="1">
+        <v>5.2552911200000003E-24</v>
+      </c>
+      <c r="E25" s="1">
+        <v>1.2804074500000001E-4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>23</v>
+      </c>
+      <c r="B26" t="s">
+        <v>48</v>
+      </c>
+      <c r="C26" s="2">
+        <v>20341.599099999999</v>
+      </c>
+      <c r="D26" s="1">
+        <v>0</v>
+      </c>
+      <c r="E26" s="1">
+        <v>1.2990199399999999E-3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>24</v>
+      </c>
+      <c r="B27" t="s">
+        <v>51</v>
+      </c>
+      <c r="C27" s="2">
+        <v>3273.3701799999999</v>
+      </c>
+      <c r="D27" s="1">
+        <v>0</v>
+      </c>
+      <c r="E27" s="1">
+        <v>3.7205022200000001E-3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>25</v>
+      </c>
+      <c r="B28" t="s">
+        <v>47</v>
+      </c>
+      <c r="C28" s="2">
+        <v>5146.6154200000001</v>
+      </c>
+      <c r="D28" s="1">
+        <v>0</v>
+      </c>
+      <c r="E28" s="1">
+        <v>1.29971556E-3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>26</v>
+      </c>
+      <c r="B29" t="s">
+        <v>49</v>
+      </c>
+      <c r="C29" s="2">
+        <v>21005.554499999998</v>
+      </c>
+      <c r="D29" s="1">
+        <v>0</v>
+      </c>
+      <c r="E29" s="1">
+        <v>6.63589657E-3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>27</v>
+      </c>
+      <c r="B30" t="s">
+        <v>52</v>
+      </c>
+      <c r="C30" s="2">
+        <v>157996.83799999999</v>
+      </c>
+      <c r="D30" s="1">
+        <v>0</v>
+      </c>
+      <c r="E30" s="1">
+        <v>2.8752784700000002E-4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>28</v>
+      </c>
+      <c r="B31" t="s">
+        <v>53</v>
+      </c>
+      <c r="C31" s="2">
+        <v>90764.6</v>
+      </c>
+      <c r="D31" s="1">
+        <v>0</v>
+      </c>
+      <c r="E31" s="1">
+        <v>1.00918102E-4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>29</v>
+      </c>
+      <c r="B32" t="s">
+        <v>57</v>
+      </c>
+      <c r="C32" s="2">
+        <v>11410.6036</v>
+      </c>
+      <c r="D32" s="1">
+        <v>0</v>
+      </c>
+      <c r="E32" s="1">
+        <v>2.9496253599999998E-7</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>30</v>
+      </c>
+      <c r="B33" t="s">
+        <v>55</v>
+      </c>
+      <c r="C33" s="2">
+        <v>2489.97111</v>
+      </c>
+      <c r="D33" s="1">
+        <v>0</v>
+      </c>
+      <c r="E33" s="1">
+        <v>8.5578218799999994E-9</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <v>31</v>
+      </c>
+      <c r="B34" t="s">
+        <v>54</v>
+      </c>
+      <c r="C34" s="2">
+        <v>1380.7544499999999</v>
+      </c>
+      <c r="D34" s="1">
+        <v>3.1955772800000002E-302</v>
+      </c>
+      <c r="E34" s="1">
+        <v>1.60063547E-8</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <v>32</v>
+      </c>
+      <c r="B35" t="s">
+        <v>58</v>
+      </c>
+      <c r="C35" s="2">
+        <v>2312.7131899999999</v>
+      </c>
+      <c r="D35" s="1">
+        <v>0</v>
+      </c>
+      <c r="E35" s="1">
+        <v>6.0724735200000004E-8</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <v>33</v>
+      </c>
+      <c r="B36" t="s">
+        <v>56</v>
+      </c>
+      <c r="C36" s="2">
+        <v>8670.2888299999995</v>
+      </c>
+      <c r="D36" s="1">
+        <v>0</v>
+      </c>
+      <c r="E36" s="1">
+        <v>3.3441193400000002E-6</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <v>34</v>
+      </c>
+      <c r="B37" t="s">
+        <v>59</v>
+      </c>
+      <c r="C37" s="2">
+        <v>547.37168099999997</v>
+      </c>
+      <c r="D37" s="1">
+        <v>4.6963321200000002E-121</v>
+      </c>
+      <c r="E37" s="1">
+        <v>5.9786323499999996E-6</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <v>35</v>
+      </c>
+      <c r="B38" t="s">
+        <v>60</v>
+      </c>
+      <c r="C38" s="2">
+        <v>2723.0854399999998</v>
+      </c>
+      <c r="D38" s="1">
+        <v>0</v>
+      </c>
+      <c r="E38" s="1">
+        <v>2.4337853099999999E-5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <v>36</v>
+      </c>
+      <c r="B39" t="s">
+        <v>61</v>
+      </c>
+      <c r="C39" s="2">
+        <v>8702.2758900000008</v>
+      </c>
+      <c r="D39" s="1">
+        <v>0</v>
+      </c>
+      <c r="E39" s="1">
+        <v>6.8334162399999996E-5</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A40">
+        <v>37</v>
+      </c>
+      <c r="B40" t="s">
+        <v>62</v>
+      </c>
+      <c r="C40" s="2">
+        <v>3592.1202899999998</v>
+      </c>
+      <c r="D40" s="1">
+        <v>0</v>
+      </c>
+      <c r="E40" s="1">
+        <v>9.2319852800000005E-5</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <v>38</v>
+      </c>
+      <c r="B41" t="s">
+        <v>63</v>
+      </c>
+      <c r="C41" s="2">
+        <v>26996.203600000001</v>
+      </c>
+      <c r="D41" s="1">
+        <v>0</v>
+      </c>
+      <c r="E41" s="1">
+        <v>2.8999942199999998E-4</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A42">
+        <v>39</v>
+      </c>
+      <c r="B42" t="s">
+        <v>64</v>
+      </c>
+      <c r="C42" s="2">
+        <v>45435.158000000003</v>
+      </c>
+      <c r="D42" s="1">
+        <v>0</v>
+      </c>
+      <c r="E42" s="1">
+        <v>4.9458860899999997E-4</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A43">
+        <v>40</v>
+      </c>
+      <c r="B43" t="s">
+        <v>65</v>
+      </c>
+      <c r="C43" s="2">
+        <v>42671.335500000001</v>
+      </c>
+      <c r="D43" s="1">
+        <v>0</v>
+      </c>
+      <c r="E43" s="1">
+        <v>7.6831112199999998E-4</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A44">
+        <v>41</v>
+      </c>
+      <c r="B44" t="s">
+        <v>66</v>
+      </c>
+      <c r="C44" s="2">
+        <v>53099.542399999998</v>
+      </c>
+      <c r="D44" s="1">
+        <v>0</v>
+      </c>
+      <c r="E44" s="1">
+        <v>7.75534007E-4</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A45">
+        <v>42</v>
+      </c>
+      <c r="B45" t="s">
+        <v>67</v>
+      </c>
+      <c r="C45" s="2">
+        <v>73489.692999999999</v>
+      </c>
+      <c r="D45" s="1">
+        <v>0</v>
+      </c>
+      <c r="E45" s="1">
+        <v>1.38215834E-3</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A46">
+        <v>43</v>
+      </c>
+      <c r="B46" t="s">
+        <v>68</v>
+      </c>
+      <c r="C46" s="2">
+        <v>65472.628199999999</v>
+      </c>
+      <c r="D46" s="1">
+        <v>0</v>
+      </c>
+      <c r="E46" s="1">
+        <v>1.2636561300000001E-3</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A47">
+        <v>44</v>
+      </c>
+      <c r="B47" t="s">
+        <v>69</v>
+      </c>
+      <c r="C47" s="2">
+        <v>58813.2235</v>
+      </c>
+      <c r="D47" s="1">
+        <v>0</v>
+      </c>
+      <c r="E47" s="1">
+        <v>1.4072254599999999E-3</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A48">
+        <v>45</v>
+      </c>
+      <c r="B48" t="s">
+        <v>70</v>
+      </c>
+      <c r="C48" s="2">
+        <v>16729.9067</v>
+      </c>
+      <c r="D48" s="1">
+        <v>0</v>
+      </c>
+      <c r="E48" s="1">
+        <v>7.4102290799999996E-5</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A49">
+        <v>46</v>
+      </c>
+      <c r="B49" t="s">
+        <v>71</v>
+      </c>
+      <c r="C49" s="2">
+        <v>196577.79800000001</v>
+      </c>
+      <c r="D49" s="1">
+        <v>0</v>
+      </c>
+      <c r="E49" s="1">
+        <v>1.4409861299999999E-3</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A50">
+        <v>47</v>
+      </c>
+      <c r="B50" t="s">
+        <v>72</v>
+      </c>
+      <c r="C50" s="2">
+        <v>451045.11599999998</v>
+      </c>
+      <c r="D50" s="1">
+        <v>0</v>
+      </c>
+      <c r="E50" s="1">
+        <v>4.2368620699999998E-3</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A51">
+        <v>48</v>
+      </c>
+      <c r="B51" t="s">
+        <v>73</v>
+      </c>
+      <c r="C51" s="2">
+        <v>462861.65899999999</v>
+      </c>
+      <c r="D51" s="1">
+        <v>0</v>
+      </c>
+      <c r="E51" s="1">
+        <v>5.6225218500000002E-3</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A52">
+        <v>49</v>
+      </c>
+      <c r="B52" t="s">
+        <v>74</v>
+      </c>
+      <c r="C52" s="2">
+        <v>359933.02500000002</v>
+      </c>
+      <c r="D52" s="1">
+        <v>0</v>
+      </c>
+      <c r="E52" s="1">
+        <v>3.5541517499999998E-3</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A53">
+        <v>50</v>
+      </c>
+      <c r="B53" t="s">
+        <v>75</v>
+      </c>
+      <c r="C53" s="2">
+        <v>232102.94200000001</v>
+      </c>
+      <c r="D53" s="1">
+        <v>0</v>
+      </c>
+      <c r="E53" s="1">
+        <v>9.2769531500000002E-4</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="E3:E53">
+    <cfRule type="dataBar" priority="1">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF638EC6"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{F8C02698-FC14-4905-AB3C-FD57C620A0FC}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
+      <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{F8C02698-FC14-4905-AB3C-FD57C620A0FC}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FF638EC6"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>E3:E53</xm:sqref>
+        </x14:conditionalFormatting>
+      </x14:conditionalFormattings>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added graph for recursive feature selection using xgboost, updated transformations to include hour of the day in the feature set, added gamma to xgb parameters
</commit_message>
<xml_diff>
--- a/hackerearth_ml3_adclick/analysis_graphs/feature_selection.xlsx
+++ b/hackerearth_ml3_adclick/analysis_graphs/feature_selection.xlsx
@@ -9,13 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3648" yWindow="0" windowWidth="22104" windowHeight="11016" activeTab="1"/>
+    <workbookView xWindow="4536" yWindow="0" windowWidth="22104" windowHeight="11016" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="81">
   <si>
     <t>chi square values</t>
   </si>
@@ -253,6 +253,21 @@
   </si>
   <si>
     <t>datetime_hour_23</t>
+  </si>
+  <si>
+    <t>Train Accuracy</t>
+  </si>
+  <si>
+    <t>Test Accuracy</t>
+  </si>
+  <si>
+    <t>Train AUC</t>
+  </si>
+  <si>
+    <t>Test AUC</t>
+  </si>
+  <si>
+    <t>num_features</t>
   </si>
 </sst>
 </file>
@@ -348,6 +363,1618 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$R$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Train Accuracy</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$R$4:$R$53</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="50"/>
+                <c:pt idx="0">
+                  <c:v>0.843245930408</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.87025261762499995</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.88883665984799998</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.95647516651599995</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.96153141244399998</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.97700402828300004</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.97954235965100001</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.98106459877700003</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.98223073080800005</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.98322070852999999</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.98373445236400003</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.98378478216700005</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.98378430735699995</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.98447752916800002</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.98492574929700005</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.98530749610199997</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.98529752510299995</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.98583833307699997</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.98604629962000001</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.98618256993499998</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.98623242492800001</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.98632738681999998</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.98651920984100006</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.98669916262599999</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.98672195348000002</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.98677228328300004</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.98686439631800005</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.98696600554199998</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.98681121765799995</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.98683875660700004</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.98688813679099996</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.98683210927499998</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.98688148945800003</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.98686629555600003</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.98706619033800003</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.987123167473</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.98707568652699995</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.98710559952300003</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.98711509571199996</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.98711699495000005</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0.98720720874699996</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0.98722287745899995</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0.98718489270300003</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>0.987228575173</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>0.98720530950899998</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>0.98720103622400002</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>0.98723902098100003</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>0.98723902098100003</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>0.98723902098100003</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>0.98723902098100003</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-FFF3-4EF5-8AC4-66F75CDDF826}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$S$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Test Accuracy</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$S$4:$S$53</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="50"/>
+                <c:pt idx="0">
+                  <c:v>0.93368573078700001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.95479909473000002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.95479909473000002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.93905572751599997</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.93905572751599997</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.97498230735199998</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.97155747206499998</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.97155747206499998</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.97291521287600002</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.97369459564799998</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.97369459564799998</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.97369459564799998</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.97369459564799998</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.97507046164</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.97563646160200002</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.97593058385300002</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.97572049653100001</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.97580617920400003</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.97609947758299997</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.97636723593499997</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.97644962312000005</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.97642902632399997</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.97643561729799999</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.976413372758</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.97645291860700001</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.97660451102800006</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.97663087492699996</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.97665394333900002</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.97637053142200003</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.97640101468100005</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.97631533200800003</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.97630709328900001</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.97625271774699995</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.97630544554599996</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.97677093314200003</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.97683437127499995</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.97672562018999998</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.97677010926999996</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.97679729704100005</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.97684837709600003</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0.97693241202500003</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0.97697772497699997</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0.97697854884900004</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>0.97699337854199997</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>0.97697607723299995</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>0.976975253361</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>0.97700491274800005</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>0.97700573662000001</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>0.97700573662000001</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>0.97700573662000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-FFF3-4EF5-8AC4-66F75CDDF826}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$T$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Train AUC</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$T$4:$T$53</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="50"/>
+                <c:pt idx="0">
+                  <c:v>0.85467039594299998</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.92956314024599995</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.96284855209700004</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.98565080177800002</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.99148937056599995</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.99632920850100004</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.99701703813499998</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.99729732228300005</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.99752016309400005</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.99768440002600001</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.99773545768600003</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.99774946655300001</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.99775392674800001</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.997931028873</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.99799702938199997</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.99807331809599997</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.99809546760900003</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.99819989526599995</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.99824842415000004</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.99830770806900004</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.99833609573000004</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.99836596037500003</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.99839624219699996</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.99842318852599998</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.99843850188899996</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.99845822891299996</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.99847154337999999</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.99847782671200003</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.99847596568300001</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.99848715279599998</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.99849655613900001</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.99850420203599999</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.99851106346499996</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.99852088689700003</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.99855190076300004</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.99855874864600003</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.99856298435699997</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.99856707524400001</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.99856885442599996</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.99857857288100005</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0.99858307851100003</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0.99858310941700001</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0.99858237723200005</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>0.99859817549499996</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>0.99859541853</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>0.99859537018800004</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>0.99859484021300005</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>0.99859482016900003</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>0.99859482016900003</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>0.99859482016900003</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-FFF3-4EF5-8AC4-66F75CDDF826}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$U$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Test AUC</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$U$4:$U$53</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="50"/>
+                <c:pt idx="0">
+                  <c:v>0.72542439943500003</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.81480785945400003</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.86924317155499997</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.91325669602799997</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.925368121185</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.94696781457699997</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.953061519252</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.95435934715399995</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.95579083461100001</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.95601898882400005</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.95603501446899997</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.95609857946099996</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.95608873803200001</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.95605589448200001</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.95728613939499996</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.95872860539500004</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.95900740006499996</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.95892995053800001</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.96020199109299997</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.96144696085000003</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.96151655890400001</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.96161012516099997</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.96169604689800003</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.96169381940599996</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.96173966119700005</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.96265684828599996</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.96274052831099999</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.96275508489600004</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.96279438225900005</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.962994499271</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.96306779738500004</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.96321921190600002</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.96314448851000001</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.96357944029300002</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.96428204436099996</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.964374077803</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.96448003282299999</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.96457356507600001</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.96454419940400005</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.964878595083</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0.96480241981899995</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0.96479472005800004</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0.96477735850400004</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>0.96502097710000001</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>0.96494418543100002</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>0.96494393436600001</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>0.96491219942100004</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>0.96490981200699999</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>0.96490981200699999</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>0.96490981200699999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-FFF3-4EF5-8AC4-66F75CDDF826}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="244271328"/>
+        <c:axId val="244251760"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="244271328"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="244251760"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="244251760"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1"/>
+          <c:min val="0.91"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="244271328"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>140970</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>32</xdr:col>
+      <xdr:colOff>160020</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>83820</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8A67065B-7EE1-488B-B234-2D3217AD5007}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1846,10 +3473,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I53"/>
+  <dimension ref="A1:U53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
+      <selection activeCell="AG11" sqref="AG11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1857,9 +3484,11 @@
     <col min="2" max="2" width="16.21875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.5546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.21875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
       <c r="C1" t="s">
         <v>4</v>
       </c>
@@ -1867,7 +3496,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
       <c r="C2" t="s">
         <v>0</v>
       </c>
@@ -1881,7 +3510,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>0</v>
       </c>
@@ -1903,8 +3532,35 @@
       <c r="I3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="L3">
+        <v>6</v>
+      </c>
+      <c r="M3" t="s">
+        <v>40</v>
+      </c>
+      <c r="N3" s="2">
+        <v>3922735.81</v>
+      </c>
+      <c r="O3" s="1">
+        <v>0.24401761</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>80</v>
+      </c>
+      <c r="R3" t="s">
+        <v>76</v>
+      </c>
+      <c r="S3" t="s">
+        <v>77</v>
+      </c>
+      <c r="T3" t="s">
+        <v>78</v>
+      </c>
+      <c r="U3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>1</v>
       </c>
@@ -1926,8 +3582,35 @@
       <c r="I4">
         <v>2.71</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="L4">
+        <v>12</v>
+      </c>
+      <c r="M4" t="s">
+        <v>29</v>
+      </c>
+      <c r="N4" s="2">
+        <v>2995640.15</v>
+      </c>
+      <c r="O4" s="1">
+        <v>0.123231378</v>
+      </c>
+      <c r="Q4">
+        <v>1</v>
+      </c>
+      <c r="R4">
+        <v>0.843245930408</v>
+      </c>
+      <c r="S4">
+        <v>0.93368573078700001</v>
+      </c>
+      <c r="T4">
+        <v>0.85467039594299998</v>
+      </c>
+      <c r="U4">
+        <v>0.72542439943500003</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>2</v>
       </c>
@@ -1949,8 +3632,35 @@
       <c r="I5">
         <v>3.84</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="L5">
+        <v>5</v>
+      </c>
+      <c r="M5" t="s">
+        <v>39</v>
+      </c>
+      <c r="N5" s="2">
+        <v>3402912.46</v>
+      </c>
+      <c r="O5" s="1">
+        <v>0.105516158</v>
+      </c>
+      <c r="Q5">
+        <v>2</v>
+      </c>
+      <c r="R5">
+        <v>0.87025261762499995</v>
+      </c>
+      <c r="S5">
+        <v>0.95479909473000002</v>
+      </c>
+      <c r="T5">
+        <v>0.92956314024599995</v>
+      </c>
+      <c r="U5">
+        <v>0.81480785945400003</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>3</v>
       </c>
@@ -1972,8 +3682,35 @@
       <c r="I6">
         <v>6.63</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="L6">
+        <v>7</v>
+      </c>
+      <c r="M6" t="s">
+        <v>41</v>
+      </c>
+      <c r="N6" s="2">
+        <v>1882656.23</v>
+      </c>
+      <c r="O6" s="1">
+        <v>0.102639786</v>
+      </c>
+      <c r="Q6">
+        <v>3</v>
+      </c>
+      <c r="R6">
+        <v>0.88883665984799998</v>
+      </c>
+      <c r="S6">
+        <v>0.95479909473000002</v>
+      </c>
+      <c r="T6">
+        <v>0.96284855209700004</v>
+      </c>
+      <c r="U6">
+        <v>0.86924317155499997</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>4</v>
       </c>
@@ -1995,8 +3732,35 @@
       <c r="I7">
         <v>7.88</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="L7">
+        <v>11</v>
+      </c>
+      <c r="M7" t="s">
+        <v>28</v>
+      </c>
+      <c r="N7" s="2">
+        <v>1965759.67</v>
+      </c>
+      <c r="O7" s="1">
+        <v>8.6760738000000004E-2</v>
+      </c>
+      <c r="Q7">
+        <v>4</v>
+      </c>
+      <c r="R7">
+        <v>0.95647516651599995</v>
+      </c>
+      <c r="S7">
+        <v>0.93905572751599997</v>
+      </c>
+      <c r="T7">
+        <v>0.98565080177800002</v>
+      </c>
+      <c r="U7">
+        <v>0.91325669602799997</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>5</v>
       </c>
@@ -2018,8 +3782,35 @@
       <c r="I8">
         <v>10.83</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="L8">
+        <v>17</v>
+      </c>
+      <c r="M8" t="s">
+        <v>35</v>
+      </c>
+      <c r="N8" s="2">
+        <v>728024.82400000002</v>
+      </c>
+      <c r="O8" s="1">
+        <v>7.1191111700000004E-2</v>
+      </c>
+      <c r="Q8">
+        <v>5</v>
+      </c>
+      <c r="R8">
+        <v>0.96153141244399998</v>
+      </c>
+      <c r="S8">
+        <v>0.93905572751599997</v>
+      </c>
+      <c r="T8">
+        <v>0.99148937056599995</v>
+      </c>
+      <c r="U8">
+        <v>0.925368121185</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>6</v>
       </c>
@@ -2035,8 +3826,35 @@
       <c r="E9" s="1">
         <v>0.24401761</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="L9">
+        <v>19</v>
+      </c>
+      <c r="M9" t="s">
+        <v>37</v>
+      </c>
+      <c r="N9" s="2">
+        <v>1955934.32</v>
+      </c>
+      <c r="O9" s="1">
+        <v>5.9929367800000001E-2</v>
+      </c>
+      <c r="Q9">
+        <v>6</v>
+      </c>
+      <c r="R9">
+        <v>0.97700402828300004</v>
+      </c>
+      <c r="S9">
+        <v>0.97498230735199998</v>
+      </c>
+      <c r="T9">
+        <v>0.99632920850100004</v>
+      </c>
+      <c r="U9">
+        <v>0.94696781457699997</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>7</v>
       </c>
@@ -2052,8 +3870,35 @@
       <c r="E10" s="1">
         <v>0.102639786</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="L10">
+        <v>4</v>
+      </c>
+      <c r="M10" t="s">
+        <v>38</v>
+      </c>
+      <c r="N10" s="2">
+        <v>1433877.96</v>
+      </c>
+      <c r="O10" s="1">
+        <v>5.1081965E-2</v>
+      </c>
+      <c r="Q10">
+        <v>7</v>
+      </c>
+      <c r="R10">
+        <v>0.97954235965100001</v>
+      </c>
+      <c r="S10">
+        <v>0.97155747206499998</v>
+      </c>
+      <c r="T10">
+        <v>0.99701703813499998</v>
+      </c>
+      <c r="U10">
+        <v>0.953061519252</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>8</v>
       </c>
@@ -2069,8 +3914,35 @@
       <c r="E11" s="1">
         <v>1.59798458E-2</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="L11">
+        <v>13</v>
+      </c>
+      <c r="M11" t="s">
+        <v>30</v>
+      </c>
+      <c r="N11" s="2">
+        <v>139916.91099999999</v>
+      </c>
+      <c r="O11" s="1">
+        <v>5.0439913699999998E-2</v>
+      </c>
+      <c r="Q11">
+        <v>8</v>
+      </c>
+      <c r="R11">
+        <v>0.98106459877700003</v>
+      </c>
+      <c r="S11">
+        <v>0.97155747206499998</v>
+      </c>
+      <c r="T11">
+        <v>0.99729732228300005</v>
+      </c>
+      <c r="U11">
+        <v>0.95435934715399995</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>9</v>
       </c>
@@ -2086,8 +3958,35 @@
       <c r="E12" s="1">
         <v>1.5661713000000001E-2</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="L12">
+        <v>18</v>
+      </c>
+      <c r="M12" t="s">
+        <v>36</v>
+      </c>
+      <c r="N12" s="2">
+        <v>16895.480299999999</v>
+      </c>
+      <c r="O12" s="1">
+        <v>2.0059922000000001E-2</v>
+      </c>
+      <c r="Q12">
+        <v>9</v>
+      </c>
+      <c r="R12">
+        <v>0.98223073080800005</v>
+      </c>
+      <c r="S12">
+        <v>0.97291521287600002</v>
+      </c>
+      <c r="T12">
+        <v>0.99752016309400005</v>
+      </c>
+      <c r="U12">
+        <v>0.95579083461100001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>10</v>
       </c>
@@ -2103,8 +4002,35 @@
       <c r="E13" s="1">
         <v>3.9819249200000002E-3</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="L13">
+        <v>8</v>
+      </c>
+      <c r="M13" t="s">
+        <v>42</v>
+      </c>
+      <c r="N13" s="2">
+        <v>182854.152</v>
+      </c>
+      <c r="O13" s="1">
+        <v>1.59798458E-2</v>
+      </c>
+      <c r="Q13">
+        <v>10</v>
+      </c>
+      <c r="R13">
+        <v>0.98322070852999999</v>
+      </c>
+      <c r="S13">
+        <v>0.97369459564799998</v>
+      </c>
+      <c r="T13">
+        <v>0.99768440002600001</v>
+      </c>
+      <c r="U13">
+        <v>0.95601898882400005</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>11</v>
       </c>
@@ -2120,8 +4046,35 @@
       <c r="E14" s="1">
         <v>8.6760738000000004E-2</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="L14">
+        <v>9</v>
+      </c>
+      <c r="M14" t="s">
+        <v>43</v>
+      </c>
+      <c r="N14" s="2">
+        <v>184865.79199999999</v>
+      </c>
+      <c r="O14" s="1">
+        <v>1.5661713000000001E-2</v>
+      </c>
+      <c r="Q14">
+        <v>11</v>
+      </c>
+      <c r="R14">
+        <v>0.98373445236400003</v>
+      </c>
+      <c r="S14">
+        <v>0.97369459564799998</v>
+      </c>
+      <c r="T14">
+        <v>0.99773545768600003</v>
+      </c>
+      <c r="U14">
+        <v>0.95603501446899997</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>12</v>
       </c>
@@ -2137,8 +4090,35 @@
       <c r="E15" s="1">
         <v>0.123231378</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="L15">
+        <v>16</v>
+      </c>
+      <c r="M15" t="s">
+        <v>34</v>
+      </c>
+      <c r="N15" s="2">
+        <v>90.685528700000006</v>
+      </c>
+      <c r="O15" s="1">
+        <v>1.17057789E-2</v>
+      </c>
+      <c r="Q15">
+        <v>12</v>
+      </c>
+      <c r="R15">
+        <v>0.98378478216700005</v>
+      </c>
+      <c r="S15">
+        <v>0.97369459564799998</v>
+      </c>
+      <c r="T15">
+        <v>0.99774946655300001</v>
+      </c>
+      <c r="U15">
+        <v>0.95609857946099996</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>13</v>
       </c>
@@ -2154,8 +4134,35 @@
       <c r="E16" s="1">
         <v>5.0439913699999998E-2</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="L16">
+        <v>26</v>
+      </c>
+      <c r="M16" t="s">
+        <v>49</v>
+      </c>
+      <c r="N16" s="2">
+        <v>21005.554499999998</v>
+      </c>
+      <c r="O16" s="1">
+        <v>6.63589657E-3</v>
+      </c>
+      <c r="Q16">
+        <v>13</v>
+      </c>
+      <c r="R16">
+        <v>0.98378430735699995</v>
+      </c>
+      <c r="S16">
+        <v>0.97369459564799998</v>
+      </c>
+      <c r="T16">
+        <v>0.99775392674800001</v>
+      </c>
+      <c r="U16">
+        <v>0.95608873803200001</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>14</v>
       </c>
@@ -2171,8 +4178,35 @@
       <c r="E17" s="1">
         <v>6.3685785099999997E-4</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="L17">
+        <v>48</v>
+      </c>
+      <c r="M17" t="s">
+        <v>73</v>
+      </c>
+      <c r="N17" s="2">
+        <v>462861.65899999999</v>
+      </c>
+      <c r="O17" s="1">
+        <v>5.6225218500000002E-3</v>
+      </c>
+      <c r="Q17">
+        <v>14</v>
+      </c>
+      <c r="R17">
+        <v>0.98447752916800002</v>
+      </c>
+      <c r="S17">
+        <v>0.97507046164</v>
+      </c>
+      <c r="T17">
+        <v>0.997931028873</v>
+      </c>
+      <c r="U17">
+        <v>0.95605589448200001</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>15</v>
       </c>
@@ -2188,8 +4222,35 @@
       <c r="E18" s="1">
         <v>2.9022666399999999E-4</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="L18">
+        <v>47</v>
+      </c>
+      <c r="M18" t="s">
+        <v>72</v>
+      </c>
+      <c r="N18" s="2">
+        <v>451045.11599999998</v>
+      </c>
+      <c r="O18" s="1">
+        <v>4.2368620699999998E-3</v>
+      </c>
+      <c r="Q18">
+        <v>15</v>
+      </c>
+      <c r="R18">
+        <v>0.98492574929700005</v>
+      </c>
+      <c r="S18">
+        <v>0.97563646160200002</v>
+      </c>
+      <c r="T18">
+        <v>0.99799702938199997</v>
+      </c>
+      <c r="U18">
+        <v>0.95728613939499996</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>16</v>
       </c>
@@ -2205,8 +4266,35 @@
       <c r="E19" s="1">
         <v>1.17057789E-2</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="L19">
+        <v>10</v>
+      </c>
+      <c r="M19" t="s">
+        <v>44</v>
+      </c>
+      <c r="N19" s="2">
+        <v>549.83858599999996</v>
+      </c>
+      <c r="O19" s="1">
+        <v>3.9819249200000002E-3</v>
+      </c>
+      <c r="Q19">
+        <v>16</v>
+      </c>
+      <c r="R19">
+        <v>0.98530749610199997</v>
+      </c>
+      <c r="S19">
+        <v>0.97593058385300002</v>
+      </c>
+      <c r="T19">
+        <v>0.99807331809599997</v>
+      </c>
+      <c r="U19">
+        <v>0.95872860539500004</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>17</v>
       </c>
@@ -2222,8 +4310,35 @@
       <c r="E20" s="1">
         <v>7.1191111700000004E-2</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="L20">
+        <v>24</v>
+      </c>
+      <c r="M20" t="s">
+        <v>51</v>
+      </c>
+      <c r="N20" s="2">
+        <v>3273.3701799999999</v>
+      </c>
+      <c r="O20" s="1">
+        <v>3.7205022200000001E-3</v>
+      </c>
+      <c r="Q20">
+        <v>17</v>
+      </c>
+      <c r="R20">
+        <v>0.98529752510299995</v>
+      </c>
+      <c r="S20">
+        <v>0.97572049653100001</v>
+      </c>
+      <c r="T20">
+        <v>0.99809546760900003</v>
+      </c>
+      <c r="U20">
+        <v>0.95900740006499996</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>18</v>
       </c>
@@ -2239,8 +4354,35 @@
       <c r="E21" s="1">
         <v>2.0059922000000001E-2</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="L21">
+        <v>49</v>
+      </c>
+      <c r="M21" t="s">
+        <v>74</v>
+      </c>
+      <c r="N21" s="2">
+        <v>359933.02500000002</v>
+      </c>
+      <c r="O21" s="1">
+        <v>3.5541517499999998E-3</v>
+      </c>
+      <c r="Q21">
+        <v>18</v>
+      </c>
+      <c r="R21">
+        <v>0.98583833307699997</v>
+      </c>
+      <c r="S21">
+        <v>0.97580617920400003</v>
+      </c>
+      <c r="T21">
+        <v>0.99819989526599995</v>
+      </c>
+      <c r="U21">
+        <v>0.95892995053800001</v>
+      </c>
+    </row>
+    <row r="22" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>19</v>
       </c>
@@ -2256,8 +4398,35 @@
       <c r="E22" s="1">
         <v>5.9929367800000001E-2</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="L22">
+        <v>46</v>
+      </c>
+      <c r="M22" t="s">
+        <v>71</v>
+      </c>
+      <c r="N22" s="2">
+        <v>196577.79800000001</v>
+      </c>
+      <c r="O22" s="1">
+        <v>1.4409861299999999E-3</v>
+      </c>
+      <c r="Q22">
+        <v>19</v>
+      </c>
+      <c r="R22">
+        <v>0.98604629962000001</v>
+      </c>
+      <c r="S22">
+        <v>0.97609947758299997</v>
+      </c>
+      <c r="T22">
+        <v>0.99824842415000004</v>
+      </c>
+      <c r="U22">
+        <v>0.96020199109299997</v>
+      </c>
+    </row>
+    <row r="23" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>20</v>
       </c>
@@ -2273,8 +4442,35 @@
       <c r="E23" s="1">
         <v>5.3523122100000004E-4</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="L23">
+        <v>44</v>
+      </c>
+      <c r="M23" t="s">
+        <v>69</v>
+      </c>
+      <c r="N23" s="2">
+        <v>58813.2235</v>
+      </c>
+      <c r="O23" s="1">
+        <v>1.4072254599999999E-3</v>
+      </c>
+      <c r="Q23">
+        <v>20</v>
+      </c>
+      <c r="R23">
+        <v>0.98618256993499998</v>
+      </c>
+      <c r="S23">
+        <v>0.97636723593499997</v>
+      </c>
+      <c r="T23">
+        <v>0.99830770806900004</v>
+      </c>
+      <c r="U23">
+        <v>0.96144696085000003</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>21</v>
       </c>
@@ -2290,8 +4486,35 @@
       <c r="E24" s="1">
         <v>1.88174024E-4</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="L24">
+        <v>42</v>
+      </c>
+      <c r="M24" t="s">
+        <v>67</v>
+      </c>
+      <c r="N24" s="2">
+        <v>73489.692999999999</v>
+      </c>
+      <c r="O24" s="1">
+        <v>1.38215834E-3</v>
+      </c>
+      <c r="Q24">
+        <v>21</v>
+      </c>
+      <c r="R24">
+        <v>0.98623242492800001</v>
+      </c>
+      <c r="S24">
+        <v>0.97644962312000005</v>
+      </c>
+      <c r="T24">
+        <v>0.99833609573000004</v>
+      </c>
+      <c r="U24">
+        <v>0.96151655890400001</v>
+      </c>
+    </row>
+    <row r="25" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>22</v>
       </c>
@@ -2307,8 +4530,35 @@
       <c r="E25" s="1">
         <v>1.2804074500000001E-4</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="L25">
+        <v>25</v>
+      </c>
+      <c r="M25" t="s">
+        <v>47</v>
+      </c>
+      <c r="N25" s="2">
+        <v>5146.6154200000001</v>
+      </c>
+      <c r="O25" s="1">
+        <v>1.29971556E-3</v>
+      </c>
+      <c r="Q25">
+        <v>22</v>
+      </c>
+      <c r="R25">
+        <v>0.98632738681999998</v>
+      </c>
+      <c r="S25">
+        <v>0.97642902632399997</v>
+      </c>
+      <c r="T25">
+        <v>0.99836596037500003</v>
+      </c>
+      <c r="U25">
+        <v>0.96161012516099997</v>
+      </c>
+    </row>
+    <row r="26" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>23</v>
       </c>
@@ -2324,8 +4574,35 @@
       <c r="E26" s="1">
         <v>1.2990199399999999E-3</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="L26">
+        <v>23</v>
+      </c>
+      <c r="M26" t="s">
+        <v>48</v>
+      </c>
+      <c r="N26" s="2">
+        <v>20341.599099999999</v>
+      </c>
+      <c r="O26" s="1">
+        <v>1.2990199399999999E-3</v>
+      </c>
+      <c r="Q26">
+        <v>23</v>
+      </c>
+      <c r="R26">
+        <v>0.98651920984100006</v>
+      </c>
+      <c r="S26">
+        <v>0.97643561729799999</v>
+      </c>
+      <c r="T26">
+        <v>0.99839624219699996</v>
+      </c>
+      <c r="U26">
+        <v>0.96169604689800003</v>
+      </c>
+    </row>
+    <row r="27" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>24</v>
       </c>
@@ -2341,8 +4618,35 @@
       <c r="E27" s="1">
         <v>3.7205022200000001E-3</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="L27">
+        <v>43</v>
+      </c>
+      <c r="M27" t="s">
+        <v>68</v>
+      </c>
+      <c r="N27" s="2">
+        <v>65472.628199999999</v>
+      </c>
+      <c r="O27" s="1">
+        <v>1.2636561300000001E-3</v>
+      </c>
+      <c r="Q27">
+        <v>24</v>
+      </c>
+      <c r="R27">
+        <v>0.98669916262599999</v>
+      </c>
+      <c r="S27">
+        <v>0.976413372758</v>
+      </c>
+      <c r="T27">
+        <v>0.99842318852599998</v>
+      </c>
+      <c r="U27">
+        <v>0.96169381940599996</v>
+      </c>
+    </row>
+    <row r="28" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>25</v>
       </c>
@@ -2358,8 +4662,35 @@
       <c r="E28" s="1">
         <v>1.29971556E-3</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="L28">
+        <v>50</v>
+      </c>
+      <c r="M28" t="s">
+        <v>75</v>
+      </c>
+      <c r="N28" s="2">
+        <v>232102.94200000001</v>
+      </c>
+      <c r="O28" s="1">
+        <v>9.2769531500000002E-4</v>
+      </c>
+      <c r="Q28">
+        <v>25</v>
+      </c>
+      <c r="R28">
+        <v>0.98672195348000002</v>
+      </c>
+      <c r="S28">
+        <v>0.97645291860700001</v>
+      </c>
+      <c r="T28">
+        <v>0.99843850188899996</v>
+      </c>
+      <c r="U28">
+        <v>0.96173966119700005</v>
+      </c>
+    </row>
+    <row r="29" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>26</v>
       </c>
@@ -2375,8 +4706,35 @@
       <c r="E29" s="1">
         <v>6.63589657E-3</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="L29">
+        <v>41</v>
+      </c>
+      <c r="M29" t="s">
+        <v>66</v>
+      </c>
+      <c r="N29" s="2">
+        <v>53099.542399999998</v>
+      </c>
+      <c r="O29" s="1">
+        <v>7.75534007E-4</v>
+      </c>
+      <c r="Q29">
+        <v>26</v>
+      </c>
+      <c r="R29">
+        <v>0.98677228328300004</v>
+      </c>
+      <c r="S29">
+        <v>0.97660451102800006</v>
+      </c>
+      <c r="T29">
+        <v>0.99845822891299996</v>
+      </c>
+      <c r="U29">
+        <v>0.96265684828599996</v>
+      </c>
+    </row>
+    <row r="30" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>27</v>
       </c>
@@ -2392,8 +4750,35 @@
       <c r="E30" s="1">
         <v>2.8752784700000002E-4</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="L30">
+        <v>40</v>
+      </c>
+      <c r="M30" t="s">
+        <v>65</v>
+      </c>
+      <c r="N30" s="2">
+        <v>42671.335500000001</v>
+      </c>
+      <c r="O30" s="1">
+        <v>7.6831112199999998E-4</v>
+      </c>
+      <c r="Q30">
+        <v>27</v>
+      </c>
+      <c r="R30">
+        <v>0.98686439631800005</v>
+      </c>
+      <c r="S30">
+        <v>0.97663087492699996</v>
+      </c>
+      <c r="T30">
+        <v>0.99847154337999999</v>
+      </c>
+      <c r="U30">
+        <v>0.96274052831099999</v>
+      </c>
+    </row>
+    <row r="31" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>28</v>
       </c>
@@ -2409,8 +4794,35 @@
       <c r="E31" s="1">
         <v>1.00918102E-4</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="L31">
+        <v>14</v>
+      </c>
+      <c r="M31" t="s">
+        <v>31</v>
+      </c>
+      <c r="N31" s="2">
+        <v>53.453002599999998</v>
+      </c>
+      <c r="O31" s="1">
+        <v>6.3685785099999997E-4</v>
+      </c>
+      <c r="Q31">
+        <v>28</v>
+      </c>
+      <c r="R31">
+        <v>0.98696600554199998</v>
+      </c>
+      <c r="S31">
+        <v>0.97665394333900002</v>
+      </c>
+      <c r="T31">
+        <v>0.99847782671200003</v>
+      </c>
+      <c r="U31">
+        <v>0.96275508489600004</v>
+      </c>
+    </row>
+    <row r="32" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>29</v>
       </c>
@@ -2426,8 +4838,35 @@
       <c r="E32" s="1">
         <v>2.9496253599999998E-7</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="L32">
+        <v>20</v>
+      </c>
+      <c r="M32" t="s">
+        <v>45</v>
+      </c>
+      <c r="N32" s="2">
+        <v>2939.2909100000002</v>
+      </c>
+      <c r="O32" s="1">
+        <v>5.3523122100000004E-4</v>
+      </c>
+      <c r="Q32">
+        <v>29</v>
+      </c>
+      <c r="R32">
+        <v>0.98681121765799995</v>
+      </c>
+      <c r="S32">
+        <v>0.97637053142200003</v>
+      </c>
+      <c r="T32">
+        <v>0.99847596568300001</v>
+      </c>
+      <c r="U32">
+        <v>0.96279438225900005</v>
+      </c>
+    </row>
+    <row r="33" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>30</v>
       </c>
@@ -2443,8 +4882,35 @@
       <c r="E33" s="1">
         <v>8.5578218799999994E-9</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="L33">
+        <v>39</v>
+      </c>
+      <c r="M33" t="s">
+        <v>64</v>
+      </c>
+      <c r="N33" s="2">
+        <v>45435.158000000003</v>
+      </c>
+      <c r="O33" s="1">
+        <v>4.9458860899999997E-4</v>
+      </c>
+      <c r="Q33">
+        <v>30</v>
+      </c>
+      <c r="R33">
+        <v>0.98683875660700004</v>
+      </c>
+      <c r="S33">
+        <v>0.97640101468100005</v>
+      </c>
+      <c r="T33">
+        <v>0.99848715279599998</v>
+      </c>
+      <c r="U33">
+        <v>0.962994499271</v>
+      </c>
+    </row>
+    <row r="34" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>31</v>
       </c>
@@ -2460,8 +4926,35 @@
       <c r="E34" s="1">
         <v>1.60063547E-8</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="L34">
+        <v>15</v>
+      </c>
+      <c r="M34" t="s">
+        <v>32</v>
+      </c>
+      <c r="N34" s="2">
+        <v>55.359001300000003</v>
+      </c>
+      <c r="O34" s="1">
+        <v>2.9022666399999999E-4</v>
+      </c>
+      <c r="Q34">
+        <v>31</v>
+      </c>
+      <c r="R34">
+        <v>0.98688813679099996</v>
+      </c>
+      <c r="S34">
+        <v>0.97631533200800003</v>
+      </c>
+      <c r="T34">
+        <v>0.99849655613900001</v>
+      </c>
+      <c r="U34">
+        <v>0.96306779738500004</v>
+      </c>
+    </row>
+    <row r="35" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>32</v>
       </c>
@@ -2477,8 +4970,35 @@
       <c r="E35" s="1">
         <v>6.0724735200000004E-8</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="L35">
+        <v>38</v>
+      </c>
+      <c r="M35" t="s">
+        <v>63</v>
+      </c>
+      <c r="N35" s="2">
+        <v>26996.203600000001</v>
+      </c>
+      <c r="O35" s="1">
+        <v>2.8999942199999998E-4</v>
+      </c>
+      <c r="Q35">
+        <v>32</v>
+      </c>
+      <c r="R35">
+        <v>0.98683210927499998</v>
+      </c>
+      <c r="S35">
+        <v>0.97630709328900001</v>
+      </c>
+      <c r="T35">
+        <v>0.99850420203599999</v>
+      </c>
+      <c r="U35">
+        <v>0.96321921190600002</v>
+      </c>
+    </row>
+    <row r="36" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>33</v>
       </c>
@@ -2494,8 +5014,35 @@
       <c r="E36" s="1">
         <v>3.3441193400000002E-6</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="L36">
+        <v>27</v>
+      </c>
+      <c r="M36" t="s">
+        <v>52</v>
+      </c>
+      <c r="N36" s="2">
+        <v>157996.83799999999</v>
+      </c>
+      <c r="O36" s="1">
+        <v>2.8752784700000002E-4</v>
+      </c>
+      <c r="Q36">
+        <v>33</v>
+      </c>
+      <c r="R36">
+        <v>0.98688148945800003</v>
+      </c>
+      <c r="S36">
+        <v>0.97625271774699995</v>
+      </c>
+      <c r="T36">
+        <v>0.99851106346499996</v>
+      </c>
+      <c r="U36">
+        <v>0.96314448851000001</v>
+      </c>
+    </row>
+    <row r="37" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>34</v>
       </c>
@@ -2511,8 +5058,35 @@
       <c r="E37" s="1">
         <v>5.9786323499999996E-6</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="L37">
+        <v>2</v>
+      </c>
+      <c r="M37" t="s">
+        <v>13</v>
+      </c>
+      <c r="N37" s="2">
+        <v>367088.40100000001</v>
+      </c>
+      <c r="O37" s="1">
+        <v>2.06433299E-4</v>
+      </c>
+      <c r="Q37">
+        <v>34</v>
+      </c>
+      <c r="R37">
+        <v>0.98686629555600003</v>
+      </c>
+      <c r="S37">
+        <v>0.97630544554599996</v>
+      </c>
+      <c r="T37">
+        <v>0.99852088689700003</v>
+      </c>
+      <c r="U37">
+        <v>0.96357944029300002</v>
+      </c>
+    </row>
+    <row r="38" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>35</v>
       </c>
@@ -2528,8 +5102,35 @@
       <c r="E38" s="1">
         <v>2.4337853099999999E-5</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="L38">
+        <v>21</v>
+      </c>
+      <c r="M38" t="s">
+        <v>46</v>
+      </c>
+      <c r="N38" s="2">
+        <v>2526.0420600000002</v>
+      </c>
+      <c r="O38" s="1">
+        <v>1.88174024E-4</v>
+      </c>
+      <c r="Q38">
+        <v>35</v>
+      </c>
+      <c r="R38">
+        <v>0.98706619033800003</v>
+      </c>
+      <c r="S38">
+        <v>0.97677093314200003</v>
+      </c>
+      <c r="T38">
+        <v>0.99855190076300004</v>
+      </c>
+      <c r="U38">
+        <v>0.96428204436099996</v>
+      </c>
+    </row>
+    <row r="39" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>36</v>
       </c>
@@ -2545,8 +5146,35 @@
       <c r="E39" s="1">
         <v>6.8334162399999996E-5</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="L39">
+        <v>22</v>
+      </c>
+      <c r="M39" t="s">
+        <v>50</v>
+      </c>
+      <c r="N39" s="2">
+        <v>102.108862</v>
+      </c>
+      <c r="O39" s="1">
+        <v>1.2804074500000001E-4</v>
+      </c>
+      <c r="Q39">
+        <v>36</v>
+      </c>
+      <c r="R39">
+        <v>0.987123167473</v>
+      </c>
+      <c r="S39">
+        <v>0.97683437127499995</v>
+      </c>
+      <c r="T39">
+        <v>0.99855874864600003</v>
+      </c>
+      <c r="U39">
+        <v>0.964374077803</v>
+      </c>
+    </row>
+    <row r="40" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>37</v>
       </c>
@@ -2562,8 +5190,35 @@
       <c r="E40" s="1">
         <v>9.2319852800000005E-5</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="L40">
+        <v>28</v>
+      </c>
+      <c r="M40" t="s">
+        <v>53</v>
+      </c>
+      <c r="N40" s="2">
+        <v>90764.6</v>
+      </c>
+      <c r="O40" s="1">
+        <v>1.00918102E-4</v>
+      </c>
+      <c r="Q40">
+        <v>37</v>
+      </c>
+      <c r="R40">
+        <v>0.98707568652699995</v>
+      </c>
+      <c r="S40">
+        <v>0.97672562018999998</v>
+      </c>
+      <c r="T40">
+        <v>0.99856298435699997</v>
+      </c>
+      <c r="U40">
+        <v>0.96448003282299999</v>
+      </c>
+    </row>
+    <row r="41" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>38</v>
       </c>
@@ -2579,8 +5234,35 @@
       <c r="E41" s="1">
         <v>2.8999942199999998E-4</v>
       </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="L41">
+        <v>37</v>
+      </c>
+      <c r="M41" t="s">
+        <v>62</v>
+      </c>
+      <c r="N41" s="2">
+        <v>3592.1202899999998</v>
+      </c>
+      <c r="O41" s="1">
+        <v>9.2319852800000005E-5</v>
+      </c>
+      <c r="Q41">
+        <v>38</v>
+      </c>
+      <c r="R41">
+        <v>0.98710559952300003</v>
+      </c>
+      <c r="S41">
+        <v>0.97677010926999996</v>
+      </c>
+      <c r="T41">
+        <v>0.99856707524400001</v>
+      </c>
+      <c r="U41">
+        <v>0.96457356507600001</v>
+      </c>
+    </row>
+    <row r="42" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>39</v>
       </c>
@@ -2596,8 +5278,35 @@
       <c r="E42" s="1">
         <v>4.9458860899999997E-4</v>
       </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="L42">
+        <v>45</v>
+      </c>
+      <c r="M42" t="s">
+        <v>70</v>
+      </c>
+      <c r="N42" s="2">
+        <v>16729.9067</v>
+      </c>
+      <c r="O42" s="1">
+        <v>7.4102290799999996E-5</v>
+      </c>
+      <c r="Q42">
+        <v>39</v>
+      </c>
+      <c r="R42">
+        <v>0.98711509571199996</v>
+      </c>
+      <c r="S42">
+        <v>0.97679729704100005</v>
+      </c>
+      <c r="T42">
+        <v>0.99856885442599996</v>
+      </c>
+      <c r="U42">
+        <v>0.96454419940400005</v>
+      </c>
+    </row>
+    <row r="43" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>40</v>
       </c>
@@ -2613,8 +5322,35 @@
       <c r="E43" s="1">
         <v>7.6831112199999998E-4</v>
       </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="L43">
+        <v>36</v>
+      </c>
+      <c r="M43" t="s">
+        <v>61</v>
+      </c>
+      <c r="N43" s="2">
+        <v>8702.2758900000008</v>
+      </c>
+      <c r="O43" s="1">
+        <v>6.8334162399999996E-5</v>
+      </c>
+      <c r="Q43">
+        <v>40</v>
+      </c>
+      <c r="R43">
+        <v>0.98711699495000005</v>
+      </c>
+      <c r="S43">
+        <v>0.97684837709600003</v>
+      </c>
+      <c r="T43">
+        <v>0.99857857288100005</v>
+      </c>
+      <c r="U43">
+        <v>0.964878595083</v>
+      </c>
+    </row>
+    <row r="44" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>41</v>
       </c>
@@ -2630,8 +5366,35 @@
       <c r="E44" s="1">
         <v>7.75534007E-4</v>
       </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="L44">
+        <v>35</v>
+      </c>
+      <c r="M44" t="s">
+        <v>60</v>
+      </c>
+      <c r="N44" s="2">
+        <v>2723.0854399999998</v>
+      </c>
+      <c r="O44" s="1">
+        <v>2.4337853099999999E-5</v>
+      </c>
+      <c r="Q44">
+        <v>41</v>
+      </c>
+      <c r="R44">
+        <v>0.98720720874699996</v>
+      </c>
+      <c r="S44">
+        <v>0.97693241202500003</v>
+      </c>
+      <c r="T44">
+        <v>0.99858307851100003</v>
+      </c>
+      <c r="U44">
+        <v>0.96480241981899995</v>
+      </c>
+    </row>
+    <row r="45" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>42</v>
       </c>
@@ -2647,8 +5410,35 @@
       <c r="E45" s="1">
         <v>1.38215834E-3</v>
       </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="L45">
+        <v>0</v>
+      </c>
+      <c r="M45" t="s">
+        <v>11</v>
+      </c>
+      <c r="N45" s="2">
+        <v>355138.342</v>
+      </c>
+      <c r="O45" s="1">
+        <v>1.7337573200000001E-5</v>
+      </c>
+      <c r="Q45">
+        <v>42</v>
+      </c>
+      <c r="R45">
+        <v>0.98722287745899995</v>
+      </c>
+      <c r="S45">
+        <v>0.97697772497699997</v>
+      </c>
+      <c r="T45">
+        <v>0.99858310941700001</v>
+      </c>
+      <c r="U45">
+        <v>0.96479472005800004</v>
+      </c>
+    </row>
+    <row r="46" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>43</v>
       </c>
@@ -2664,8 +5454,35 @@
       <c r="E46" s="1">
         <v>1.2636561300000001E-3</v>
       </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="L46">
+        <v>3</v>
+      </c>
+      <c r="M46" t="s">
+        <v>14</v>
+      </c>
+      <c r="N46" s="2">
+        <v>7230137.4000000004</v>
+      </c>
+      <c r="O46" s="1">
+        <v>1.51952052E-5</v>
+      </c>
+      <c r="Q46">
+        <v>43</v>
+      </c>
+      <c r="R46">
+        <v>0.98718489270300003</v>
+      </c>
+      <c r="S46">
+        <v>0.97697854884900004</v>
+      </c>
+      <c r="T46">
+        <v>0.99858237723200005</v>
+      </c>
+      <c r="U46">
+        <v>0.96477735850400004</v>
+      </c>
+    </row>
+    <row r="47" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>44</v>
       </c>
@@ -2681,8 +5498,35 @@
       <c r="E47" s="1">
         <v>1.4072254599999999E-3</v>
       </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="L47">
+        <v>1</v>
+      </c>
+      <c r="M47" t="s">
+        <v>12</v>
+      </c>
+      <c r="N47" s="2">
+        <v>429213.31599999999</v>
+      </c>
+      <c r="O47" s="1">
+        <v>9.2234408799999997E-6</v>
+      </c>
+      <c r="Q47">
+        <v>44</v>
+      </c>
+      <c r="R47">
+        <v>0.987228575173</v>
+      </c>
+      <c r="S47">
+        <v>0.97699337854199997</v>
+      </c>
+      <c r="T47">
+        <v>0.99859817549499996</v>
+      </c>
+      <c r="U47">
+        <v>0.96502097710000001</v>
+      </c>
+    </row>
+    <row r="48" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>45</v>
       </c>
@@ -2698,8 +5542,35 @@
       <c r="E48" s="1">
         <v>7.4102290799999996E-5</v>
       </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="L48">
+        <v>34</v>
+      </c>
+      <c r="M48" t="s">
+        <v>59</v>
+      </c>
+      <c r="N48" s="2">
+        <v>547.37168099999997</v>
+      </c>
+      <c r="O48" s="1">
+        <v>5.9786323499999996E-6</v>
+      </c>
+      <c r="Q48">
+        <v>45</v>
+      </c>
+      <c r="R48">
+        <v>0.98720530950899998</v>
+      </c>
+      <c r="S48">
+        <v>0.97697607723299995</v>
+      </c>
+      <c r="T48">
+        <v>0.99859541853</v>
+      </c>
+      <c r="U48">
+        <v>0.96494418543100002</v>
+      </c>
+    </row>
+    <row r="49" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>46</v>
       </c>
@@ -2715,8 +5586,35 @@
       <c r="E49" s="1">
         <v>1.4409861299999999E-3</v>
       </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="L49">
+        <v>33</v>
+      </c>
+      <c r="M49" t="s">
+        <v>56</v>
+      </c>
+      <c r="N49" s="2">
+        <v>8670.2888299999995</v>
+      </c>
+      <c r="O49" s="1">
+        <v>3.3441193400000002E-6</v>
+      </c>
+      <c r="Q49">
+        <v>46</v>
+      </c>
+      <c r="R49">
+        <v>0.98720103622400002</v>
+      </c>
+      <c r="S49">
+        <v>0.976975253361</v>
+      </c>
+      <c r="T49">
+        <v>0.99859537018800004</v>
+      </c>
+      <c r="U49">
+        <v>0.96494393436600001</v>
+      </c>
+    </row>
+    <row r="50" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>47</v>
       </c>
@@ -2732,8 +5630,35 @@
       <c r="E50" s="1">
         <v>4.2368620699999998E-3</v>
       </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="L50">
+        <v>29</v>
+      </c>
+      <c r="M50" t="s">
+        <v>57</v>
+      </c>
+      <c r="N50" s="2">
+        <v>11410.6036</v>
+      </c>
+      <c r="O50" s="1">
+        <v>2.9496253599999998E-7</v>
+      </c>
+      <c r="Q50">
+        <v>47</v>
+      </c>
+      <c r="R50">
+        <v>0.98723902098100003</v>
+      </c>
+      <c r="S50">
+        <v>0.97700491274800005</v>
+      </c>
+      <c r="T50">
+        <v>0.99859484021300005</v>
+      </c>
+      <c r="U50">
+        <v>0.96491219942100004</v>
+      </c>
+    </row>
+    <row r="51" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>48</v>
       </c>
@@ -2749,8 +5674,35 @@
       <c r="E51" s="1">
         <v>5.6225218500000002E-3</v>
       </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="L51">
+        <v>32</v>
+      </c>
+      <c r="M51" t="s">
+        <v>58</v>
+      </c>
+      <c r="N51" s="2">
+        <v>2312.7131899999999</v>
+      </c>
+      <c r="O51" s="1">
+        <v>6.0724735200000004E-8</v>
+      </c>
+      <c r="Q51">
+        <v>48</v>
+      </c>
+      <c r="R51">
+        <v>0.98723902098100003</v>
+      </c>
+      <c r="S51">
+        <v>0.97700573662000001</v>
+      </c>
+      <c r="T51">
+        <v>0.99859482016900003</v>
+      </c>
+      <c r="U51">
+        <v>0.96490981200699999</v>
+      </c>
+    </row>
+    <row r="52" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>49</v>
       </c>
@@ -2766,8 +5718,35 @@
       <c r="E52" s="1">
         <v>3.5541517499999998E-3</v>
       </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="L52">
+        <v>31</v>
+      </c>
+      <c r="M52" t="s">
+        <v>54</v>
+      </c>
+      <c r="N52" s="2">
+        <v>1380.7544499999999</v>
+      </c>
+      <c r="O52" s="1">
+        <v>1.60063547E-8</v>
+      </c>
+      <c r="Q52">
+        <v>49</v>
+      </c>
+      <c r="R52">
+        <v>0.98723902098100003</v>
+      </c>
+      <c r="S52">
+        <v>0.97700573662000001</v>
+      </c>
+      <c r="T52">
+        <v>0.99859482016900003</v>
+      </c>
+      <c r="U52">
+        <v>0.96490981200699999</v>
+      </c>
+    </row>
+    <row r="53" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>50</v>
       </c>
@@ -2783,10 +5762,40 @@
       <c r="E53" s="1">
         <v>9.2769531500000002E-4</v>
       </c>
+      <c r="L53">
+        <v>30</v>
+      </c>
+      <c r="M53" t="s">
+        <v>55</v>
+      </c>
+      <c r="N53" s="2">
+        <v>2489.97111</v>
+      </c>
+      <c r="O53" s="1">
+        <v>8.5578218799999994E-9</v>
+      </c>
+      <c r="Q53">
+        <v>50</v>
+      </c>
+      <c r="R53">
+        <v>0.98723902098100003</v>
+      </c>
+      <c r="S53">
+        <v>0.97700573662000001</v>
+      </c>
+      <c r="T53">
+        <v>0.99859482016900003</v>
+      </c>
+      <c r="U53">
+        <v>0.96490981200699999</v>
+      </c>
     </row>
   </sheetData>
+  <sortState ref="L3:O53">
+    <sortCondition descending="1" ref="O4"/>
+  </sortState>
   <conditionalFormatting sqref="E3:E53">
-    <cfRule type="dataBar" priority="1">
+    <cfRule type="dataBar" priority="2">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -2799,7 +5808,22 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="O3:O53">
+    <cfRule type="dataBar" priority="1">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF638EC6"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{D81A343A-14E0-4882-83DE-94AEF997FBED}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
@@ -2816,6 +5840,19 @@
           </x14:cfRule>
           <xm:sqref>E3:E53</xm:sqref>
         </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{D81A343A-14E0-4882-83DE-94AEF997FBED}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FF638EC6"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>O3:O53</xm:sqref>
+        </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
   </extLst>

</xml_diff>

<commit_message>
basic codes for the baseline model without any feature engineering are complete, starting a separate folder for preparing models with feature engineering
</commit_message>
<xml_diff>
--- a/hackerearth_ml3_adclick/analysis_graphs/feature_selection.xlsx
+++ b/hackerearth_ml3_adclick/analysis_graphs/feature_selection.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="4536" yWindow="0" windowWidth="22104" windowHeight="11016" activeTab="1"/>
+    <workbookView xWindow="5424" yWindow="0" windowWidth="22104" windowHeight="11016" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2276,8 +2276,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView topLeftCell="B8" workbookViewId="0">
+      <selection activeCell="I10" sqref="G3:I29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3393,9 +3393,6 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="O3:R29">
-    <sortCondition descending="1" ref="Q3"/>
-  </sortState>
   <conditionalFormatting sqref="G3:G29">
     <cfRule type="cellIs" dxfId="1" priority="5" operator="greaterThan">
       <formula>$M$6</formula>
@@ -3475,8 +3472,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
-      <selection activeCell="AG11" sqref="AG11"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="O3" sqref="O3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
added codes for model training with the additional features, also update the model logs
</commit_message>
<xml_diff>
--- a/hackerearth_ml3_adclick/analysis_graphs/feature_selection.xlsx
+++ b/hackerearth_ml3_adclick/analysis_graphs/feature_selection.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="5424" yWindow="0" windowWidth="22104" windowHeight="11016" activeTab="1"/>
+    <workbookView xWindow="7200" yWindow="0" windowWidth="22104" windowHeight="11016" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="97">
   <si>
     <t>chi square values</t>
   </si>
@@ -268,6 +269,54 @@
   </si>
   <si>
     <t>num_features</t>
+  </si>
+  <si>
+    <t>count_merchant</t>
+  </si>
+  <si>
+    <t>num_0_merchant</t>
+  </si>
+  <si>
+    <t>num_1_merchant</t>
+  </si>
+  <si>
+    <t>click_rate_merchant</t>
+  </si>
+  <si>
+    <t>count_siteid</t>
+  </si>
+  <si>
+    <t>num_0_siteid</t>
+  </si>
+  <si>
+    <t>num_1_siteid</t>
+  </si>
+  <si>
+    <t>click_rate_siteid</t>
+  </si>
+  <si>
+    <t>count_offerid</t>
+  </si>
+  <si>
+    <t>num_0_offerid</t>
+  </si>
+  <si>
+    <t>num_1_offerid</t>
+  </si>
+  <si>
+    <t>click_rate_offerid</t>
+  </si>
+  <si>
+    <t>count_category</t>
+  </si>
+  <si>
+    <t>num_0_category</t>
+  </si>
+  <si>
+    <t>num_1_category</t>
+  </si>
+  <si>
+    <t>click_rate_category</t>
   </si>
 </sst>
 </file>
@@ -3472,8 +3521,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="O3" sqref="O3"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="R53" sqref="R53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5854,4 +5903,1948 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:P65"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="N13" sqref="N13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="16.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="17" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="C2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C3" s="2">
+        <v>145362183000</v>
+      </c>
+      <c r="D3" s="2">
+        <v>0</v>
+      </c>
+      <c r="E3" s="1">
+        <v>1.7028586399999999E-4</v>
+      </c>
+      <c r="H3" t="s">
+        <v>10</v>
+      </c>
+      <c r="I3" t="s">
+        <v>9</v>
+      </c>
+      <c r="M3" s="3">
+        <v>18</v>
+      </c>
+      <c r="N3" t="s">
+        <v>40</v>
+      </c>
+      <c r="O3" s="2">
+        <v>4107965.23</v>
+      </c>
+      <c r="P3" s="1">
+        <v>0.16364116000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C4" s="2">
+        <v>135277512000</v>
+      </c>
+      <c r="D4" s="2">
+        <v>0</v>
+      </c>
+      <c r="E4" s="1">
+        <v>1.3878911899999999E-4</v>
+      </c>
+      <c r="H4">
+        <v>0.1</v>
+      </c>
+      <c r="I4">
+        <v>2.71</v>
+      </c>
+      <c r="M4" s="3">
+        <v>11</v>
+      </c>
+      <c r="N4" t="s">
+        <v>92</v>
+      </c>
+      <c r="O4" s="2">
+        <v>1320868.29</v>
+      </c>
+      <c r="P4" s="1">
+        <v>0.107179069</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5" t="s">
+        <v>83</v>
+      </c>
+      <c r="C5" s="2">
+        <v>10571150000</v>
+      </c>
+      <c r="D5" s="2">
+        <v>0</v>
+      </c>
+      <c r="E5" s="1">
+        <v>4.2911005400000002E-4</v>
+      </c>
+      <c r="H5">
+        <v>0.05</v>
+      </c>
+      <c r="I5">
+        <v>3.84</v>
+      </c>
+      <c r="M5" s="3">
+        <v>24</v>
+      </c>
+      <c r="N5" t="s">
+        <v>29</v>
+      </c>
+      <c r="O5" s="2">
+        <v>3154640.92</v>
+      </c>
+      <c r="P5" s="1">
+        <v>9.7768163300000002E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>3</v>
+      </c>
+      <c r="B6" t="s">
+        <v>84</v>
+      </c>
+      <c r="C6" s="2">
+        <v>10846.562099999999</v>
+      </c>
+      <c r="D6" s="2">
+        <v>0</v>
+      </c>
+      <c r="E6" s="1">
+        <v>1.9942958199999999E-3</v>
+      </c>
+      <c r="H6">
+        <v>0.01</v>
+      </c>
+      <c r="I6">
+        <v>6.63</v>
+      </c>
+      <c r="M6" s="3">
+        <v>7</v>
+      </c>
+      <c r="N6" t="s">
+        <v>88</v>
+      </c>
+      <c r="O6" s="2">
+        <v>341853.92800000001</v>
+      </c>
+      <c r="P6" s="1">
+        <v>8.9458355200000006E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>4</v>
+      </c>
+      <c r="B7" t="s">
+        <v>85</v>
+      </c>
+      <c r="C7" s="2">
+        <v>6009824840000</v>
+      </c>
+      <c r="D7" s="2">
+        <v>0</v>
+      </c>
+      <c r="E7" s="1">
+        <v>3.6091218199999997E-2</v>
+      </c>
+      <c r="H7">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="I7">
+        <v>7.88</v>
+      </c>
+      <c r="M7" s="3">
+        <v>17</v>
+      </c>
+      <c r="N7" t="s">
+        <v>39</v>
+      </c>
+      <c r="O7" s="2">
+        <v>3513597.54</v>
+      </c>
+      <c r="P7" s="1">
+        <v>7.2664140700000004E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>5</v>
+      </c>
+      <c r="B8" t="s">
+        <v>86</v>
+      </c>
+      <c r="C8" s="2">
+        <v>5212092690000</v>
+      </c>
+      <c r="D8" s="2">
+        <v>0</v>
+      </c>
+      <c r="E8" s="1">
+        <v>4.5756804200000001E-2</v>
+      </c>
+      <c r="H8">
+        <v>1E-3</v>
+      </c>
+      <c r="I8">
+        <v>10.83</v>
+      </c>
+      <c r="M8" s="3">
+        <v>10</v>
+      </c>
+      <c r="N8" t="s">
+        <v>91</v>
+      </c>
+      <c r="O8" s="2">
+        <v>95364603.900000006</v>
+      </c>
+      <c r="P8" s="1">
+        <v>7.0634828100000005E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>6</v>
+      </c>
+      <c r="B9" t="s">
+        <v>87</v>
+      </c>
+      <c r="C9" s="2">
+        <v>802830051000</v>
+      </c>
+      <c r="D9" s="2">
+        <v>0</v>
+      </c>
+      <c r="E9" s="1">
+        <v>4.4015375400000001E-2</v>
+      </c>
+      <c r="M9" s="3">
+        <v>19</v>
+      </c>
+      <c r="N9" t="s">
+        <v>41</v>
+      </c>
+      <c r="O9" s="2">
+        <v>1886848.61</v>
+      </c>
+      <c r="P9" s="1">
+        <v>6.0252814500000001E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>7</v>
+      </c>
+      <c r="B10" t="s">
+        <v>88</v>
+      </c>
+      <c r="C10" s="2">
+        <v>341853.92800000001</v>
+      </c>
+      <c r="D10" s="2">
+        <v>0</v>
+      </c>
+      <c r="E10" s="1">
+        <v>8.9458355200000006E-2</v>
+      </c>
+      <c r="M10" s="3">
+        <v>31</v>
+      </c>
+      <c r="N10" t="s">
+        <v>37</v>
+      </c>
+      <c r="O10" s="2">
+        <v>2061221.22</v>
+      </c>
+      <c r="P10" s="1">
+        <v>5.2146508699999997E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>8</v>
+      </c>
+      <c r="B11" t="s">
+        <v>89</v>
+      </c>
+      <c r="C11" s="2">
+        <v>2071940000</v>
+      </c>
+      <c r="D11" s="2">
+        <v>0</v>
+      </c>
+      <c r="E11" s="1">
+        <v>2.1131549999999998E-3</v>
+      </c>
+      <c r="M11" s="3">
+        <v>5</v>
+      </c>
+      <c r="N11" t="s">
+        <v>86</v>
+      </c>
+      <c r="O11" s="2">
+        <v>5212092690000</v>
+      </c>
+      <c r="P11" s="1">
+        <v>4.5756804200000001E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>9</v>
+      </c>
+      <c r="B12" t="s">
+        <v>90</v>
+      </c>
+      <c r="C12" s="2">
+        <v>1977601580</v>
+      </c>
+      <c r="D12" s="2">
+        <v>0</v>
+      </c>
+      <c r="E12" s="1">
+        <v>3.5863257899999999E-3</v>
+      </c>
+      <c r="M12" s="3">
+        <v>6</v>
+      </c>
+      <c r="N12" t="s">
+        <v>87</v>
+      </c>
+      <c r="O12" s="2">
+        <v>802830051000</v>
+      </c>
+      <c r="P12" s="1">
+        <v>4.4015375400000001E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>10</v>
+      </c>
+      <c r="B13" t="s">
+        <v>91</v>
+      </c>
+      <c r="C13" s="2">
+        <v>95364603.900000006</v>
+      </c>
+      <c r="D13" s="2">
+        <v>0</v>
+      </c>
+      <c r="E13" s="1">
+        <v>7.0634828100000005E-2</v>
+      </c>
+      <c r="M13" s="3">
+        <v>4</v>
+      </c>
+      <c r="N13" t="s">
+        <v>85</v>
+      </c>
+      <c r="O13" s="2">
+        <v>6009824840000</v>
+      </c>
+      <c r="P13" s="1">
+        <v>3.6091218199999997E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>11</v>
+      </c>
+      <c r="B14" t="s">
+        <v>92</v>
+      </c>
+      <c r="C14" s="2">
+        <v>1320868.29</v>
+      </c>
+      <c r="D14" s="2">
+        <v>0</v>
+      </c>
+      <c r="E14" s="1">
+        <v>0.107179069</v>
+      </c>
+      <c r="M14" s="3">
+        <v>23</v>
+      </c>
+      <c r="N14" t="s">
+        <v>28</v>
+      </c>
+      <c r="O14" s="2">
+        <v>2003287.78</v>
+      </c>
+      <c r="P14" s="1">
+        <v>3.20805417E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>12</v>
+      </c>
+      <c r="B15" t="s">
+        <v>93</v>
+      </c>
+      <c r="C15" s="2">
+        <v>63670269400</v>
+      </c>
+      <c r="D15" s="2">
+        <v>0</v>
+      </c>
+      <c r="E15" s="1">
+        <v>5.9713537299999999E-5</v>
+      </c>
+      <c r="M15" s="3">
+        <v>29</v>
+      </c>
+      <c r="N15" t="s">
+        <v>35</v>
+      </c>
+      <c r="O15" s="2">
+        <v>797297.33600000001</v>
+      </c>
+      <c r="P15" s="1">
+        <v>3.1570288100000003E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>13</v>
+      </c>
+      <c r="B16" t="s">
+        <v>94</v>
+      </c>
+      <c r="C16" s="2">
+        <v>57198682700</v>
+      </c>
+      <c r="D16" s="2">
+        <v>0</v>
+      </c>
+      <c r="E16" s="1">
+        <v>4.7108162899999998E-5</v>
+      </c>
+      <c r="M16" s="3">
+        <v>16</v>
+      </c>
+      <c r="N16" t="s">
+        <v>38</v>
+      </c>
+      <c r="O16" s="2">
+        <v>1524153.15</v>
+      </c>
+      <c r="P16" s="1">
+        <v>3.1209416600000001E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>14</v>
+      </c>
+      <c r="B17" t="s">
+        <v>95</v>
+      </c>
+      <c r="C17" s="2">
+        <v>7854919520</v>
+      </c>
+      <c r="D17" s="2">
+        <v>0</v>
+      </c>
+      <c r="E17" s="1">
+        <v>8.3318041399999996E-5</v>
+      </c>
+      <c r="M17" s="3">
+        <v>25</v>
+      </c>
+      <c r="N17" t="s">
+        <v>30</v>
+      </c>
+      <c r="O17" s="2">
+        <v>170552.717</v>
+      </c>
+      <c r="P17" s="1">
+        <v>1.8429558799999999E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>15</v>
+      </c>
+      <c r="B18" t="s">
+        <v>96</v>
+      </c>
+      <c r="C18" s="2">
+        <v>5014.9482500000004</v>
+      </c>
+      <c r="D18" s="2">
+        <v>0</v>
+      </c>
+      <c r="E18" s="1">
+        <v>6.6507599400000004E-4</v>
+      </c>
+      <c r="M18">
+        <v>30</v>
+      </c>
+      <c r="N18" t="s">
+        <v>36</v>
+      </c>
+      <c r="O18" s="2">
+        <v>18706.088</v>
+      </c>
+      <c r="P18" s="1">
+        <v>5.6886576799999996E-3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>16</v>
+      </c>
+      <c r="B19" t="s">
+        <v>38</v>
+      </c>
+      <c r="C19" s="2">
+        <v>1524153.15</v>
+      </c>
+      <c r="D19" s="2">
+        <v>0</v>
+      </c>
+      <c r="E19" s="1">
+        <v>3.1209416600000001E-2</v>
+      </c>
+      <c r="M19">
+        <v>21</v>
+      </c>
+      <c r="N19" t="s">
+        <v>43</v>
+      </c>
+      <c r="O19" s="2">
+        <v>227316.22399999999</v>
+      </c>
+      <c r="P19" s="1">
+        <v>5.2112508299999999E-3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>17</v>
+      </c>
+      <c r="B20" t="s">
+        <v>39</v>
+      </c>
+      <c r="C20" s="2">
+        <v>3513597.54</v>
+      </c>
+      <c r="D20" s="2">
+        <v>0</v>
+      </c>
+      <c r="E20" s="1">
+        <v>7.2664140700000004E-2</v>
+      </c>
+      <c r="M20">
+        <v>20</v>
+      </c>
+      <c r="N20" t="s">
+        <v>42</v>
+      </c>
+      <c r="O20" s="2">
+        <v>225338.21</v>
+      </c>
+      <c r="P20" s="1">
+        <v>5.0828843199999998E-3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>18</v>
+      </c>
+      <c r="B21" t="s">
+        <v>40</v>
+      </c>
+      <c r="C21" s="2">
+        <v>4107965.23</v>
+      </c>
+      <c r="D21" s="2">
+        <v>0</v>
+      </c>
+      <c r="E21" s="1">
+        <v>0.16364116000000001</v>
+      </c>
+      <c r="M21">
+        <v>60</v>
+      </c>
+      <c r="N21" t="s">
+        <v>73</v>
+      </c>
+      <c r="O21" s="2">
+        <v>476734.81099999999</v>
+      </c>
+      <c r="P21" s="1">
+        <v>4.1012085499999998E-3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>19</v>
+      </c>
+      <c r="B22" t="s">
+        <v>41</v>
+      </c>
+      <c r="C22" s="2">
+        <v>1886848.61</v>
+      </c>
+      <c r="D22" s="2">
+        <v>0</v>
+      </c>
+      <c r="E22" s="1">
+        <v>6.0252814500000001E-2</v>
+      </c>
+      <c r="M22">
+        <v>9</v>
+      </c>
+      <c r="N22" t="s">
+        <v>90</v>
+      </c>
+      <c r="O22" s="2">
+        <v>1977601580</v>
+      </c>
+      <c r="P22" s="1">
+        <v>3.5863257899999999E-3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>20</v>
+      </c>
+      <c r="B23" t="s">
+        <v>42</v>
+      </c>
+      <c r="C23" s="2">
+        <v>225338.21</v>
+      </c>
+      <c r="D23" s="2">
+        <v>0</v>
+      </c>
+      <c r="E23" s="1">
+        <v>5.0828843199999998E-3</v>
+      </c>
+      <c r="M23">
+        <v>28</v>
+      </c>
+      <c r="N23" t="s">
+        <v>34</v>
+      </c>
+      <c r="O23" s="2">
+        <v>4165.00144</v>
+      </c>
+      <c r="P23" s="1">
+        <v>3.44867836E-3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>21</v>
+      </c>
+      <c r="B24" t="s">
+        <v>43</v>
+      </c>
+      <c r="C24" s="2">
+        <v>227316.22399999999</v>
+      </c>
+      <c r="D24" s="2">
+        <v>0</v>
+      </c>
+      <c r="E24" s="1">
+        <v>5.2112508299999999E-3</v>
+      </c>
+      <c r="M24">
+        <v>59</v>
+      </c>
+      <c r="N24" t="s">
+        <v>72</v>
+      </c>
+      <c r="O24" s="2">
+        <v>463414.08100000001</v>
+      </c>
+      <c r="P24" s="1">
+        <v>3.01429916E-3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>22</v>
+      </c>
+      <c r="B25" t="s">
+        <v>44</v>
+      </c>
+      <c r="C25" s="2">
+        <v>7203.8161499999997</v>
+      </c>
+      <c r="D25" s="2">
+        <v>0</v>
+      </c>
+      <c r="E25" s="1">
+        <v>1.36848545E-3</v>
+      </c>
+      <c r="M25">
+        <v>8</v>
+      </c>
+      <c r="N25" t="s">
+        <v>89</v>
+      </c>
+      <c r="O25" s="2">
+        <v>2071940000</v>
+      </c>
+      <c r="P25" s="1">
+        <v>2.1131549999999998E-3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>23</v>
+      </c>
+      <c r="B26" t="s">
+        <v>28</v>
+      </c>
+      <c r="C26" s="2">
+        <v>2003287.78</v>
+      </c>
+      <c r="D26" s="2">
+        <v>0</v>
+      </c>
+      <c r="E26" s="1">
+        <v>3.20805417E-2</v>
+      </c>
+      <c r="M26">
+        <v>3</v>
+      </c>
+      <c r="N26" t="s">
+        <v>84</v>
+      </c>
+      <c r="O26" s="2">
+        <v>10846.562099999999</v>
+      </c>
+      <c r="P26" s="1">
+        <v>1.9942958199999999E-3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>24</v>
+      </c>
+      <c r="B27" t="s">
+        <v>29</v>
+      </c>
+      <c r="C27" s="2">
+        <v>3154640.92</v>
+      </c>
+      <c r="D27" s="2">
+        <v>0</v>
+      </c>
+      <c r="E27" s="1">
+        <v>9.7768163300000002E-2</v>
+      </c>
+      <c r="M27">
+        <v>61</v>
+      </c>
+      <c r="N27" t="s">
+        <v>74</v>
+      </c>
+      <c r="O27" s="2">
+        <v>368657.85200000001</v>
+      </c>
+      <c r="P27" s="1">
+        <v>1.63361552E-3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>25</v>
+      </c>
+      <c r="B28" t="s">
+        <v>30</v>
+      </c>
+      <c r="C28" s="2">
+        <v>170552.717</v>
+      </c>
+      <c r="D28" s="2">
+        <v>0</v>
+      </c>
+      <c r="E28" s="1">
+        <v>1.8429558799999999E-2</v>
+      </c>
+      <c r="M28">
+        <v>55</v>
+      </c>
+      <c r="N28" t="s">
+        <v>68</v>
+      </c>
+      <c r="O28" s="2">
+        <v>68242.3989</v>
+      </c>
+      <c r="P28" s="1">
+        <v>1.5004106200000001E-3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>26</v>
+      </c>
+      <c r="B29" t="s">
+        <v>31</v>
+      </c>
+      <c r="C29" s="2">
+        <v>1723.94676</v>
+      </c>
+      <c r="D29" s="2">
+        <v>0</v>
+      </c>
+      <c r="E29" s="1">
+        <v>1.8261442199999999E-4</v>
+      </c>
+      <c r="M29">
+        <v>22</v>
+      </c>
+      <c r="N29" t="s">
+        <v>44</v>
+      </c>
+      <c r="O29" s="2">
+        <v>7203.8161499999997</v>
+      </c>
+      <c r="P29" s="1">
+        <v>1.36848545E-3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>27</v>
+      </c>
+      <c r="B30" t="s">
+        <v>32</v>
+      </c>
+      <c r="C30" s="2">
+        <v>2363.9002399999999</v>
+      </c>
+      <c r="D30" s="2">
+        <v>0</v>
+      </c>
+      <c r="E30" s="1">
+        <v>2.67400202E-4</v>
+      </c>
+      <c r="M30">
+        <v>56</v>
+      </c>
+      <c r="N30" t="s">
+        <v>69</v>
+      </c>
+      <c r="O30" s="2">
+        <v>59922.8128</v>
+      </c>
+      <c r="P30" s="1">
+        <v>1.1541742399999999E-3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>28</v>
+      </c>
+      <c r="B31" t="s">
+        <v>34</v>
+      </c>
+      <c r="C31" s="2">
+        <v>4165.00144</v>
+      </c>
+      <c r="D31" s="2">
+        <v>0</v>
+      </c>
+      <c r="E31" s="1">
+        <v>3.44867836E-3</v>
+      </c>
+      <c r="M31">
+        <v>54</v>
+      </c>
+      <c r="N31" t="s">
+        <v>67</v>
+      </c>
+      <c r="O31" s="2">
+        <v>77053.963600000003</v>
+      </c>
+      <c r="P31" s="1">
+        <v>7.1921307400000004E-4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>29</v>
+      </c>
+      <c r="B32" t="s">
+        <v>35</v>
+      </c>
+      <c r="C32" s="2">
+        <v>797297.33600000001</v>
+      </c>
+      <c r="D32" s="2">
+        <v>0</v>
+      </c>
+      <c r="E32" s="1">
+        <v>3.1570288100000003E-2</v>
+      </c>
+      <c r="M32">
+        <v>52</v>
+      </c>
+      <c r="N32" t="s">
+        <v>65</v>
+      </c>
+      <c r="O32" s="2">
+        <v>45201.678099999997</v>
+      </c>
+      <c r="P32" s="1">
+        <v>6.7452916599999998E-4</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>30</v>
+      </c>
+      <c r="B33" t="s">
+        <v>36</v>
+      </c>
+      <c r="C33" s="2">
+        <v>18706.088</v>
+      </c>
+      <c r="D33" s="2">
+        <v>0</v>
+      </c>
+      <c r="E33" s="1">
+        <v>5.6886576799999996E-3</v>
+      </c>
+      <c r="M33">
+        <v>15</v>
+      </c>
+      <c r="N33" t="s">
+        <v>96</v>
+      </c>
+      <c r="O33" s="2">
+        <v>5014.9482500000004</v>
+      </c>
+      <c r="P33" s="1">
+        <v>6.6507599400000004E-4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <v>31</v>
+      </c>
+      <c r="B34" t="s">
+        <v>37</v>
+      </c>
+      <c r="C34" s="2">
+        <v>2061221.22</v>
+      </c>
+      <c r="D34" s="2">
+        <v>0</v>
+      </c>
+      <c r="E34" s="1">
+        <v>5.2146508699999997E-2</v>
+      </c>
+      <c r="M34">
+        <v>38</v>
+      </c>
+      <c r="N34" t="s">
+        <v>49</v>
+      </c>
+      <c r="O34" s="2">
+        <v>20761.0965</v>
+      </c>
+      <c r="P34" s="1">
+        <v>6.4750826200000002E-4</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <v>32</v>
+      </c>
+      <c r="B35" t="s">
+        <v>45</v>
+      </c>
+      <c r="C35" s="2">
+        <v>4398.0275300000003</v>
+      </c>
+      <c r="D35" s="2">
+        <v>0</v>
+      </c>
+      <c r="E35" s="1">
+        <v>5.3061747400000002E-5</v>
+      </c>
+      <c r="M35">
+        <v>62</v>
+      </c>
+      <c r="N35" t="s">
+        <v>75</v>
+      </c>
+      <c r="O35" s="2">
+        <v>233485.66800000001</v>
+      </c>
+      <c r="P35" s="1">
+        <v>6.3247038699999997E-4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <v>33</v>
+      </c>
+      <c r="B36" t="s">
+        <v>46</v>
+      </c>
+      <c r="C36" s="2">
+        <v>1399.1057800000001</v>
+      </c>
+      <c r="D36" s="2">
+        <v>3.2865931900000001E-306</v>
+      </c>
+      <c r="E36" s="1">
+        <v>3.4387901200000003E-5</v>
+      </c>
+      <c r="M36">
+        <v>58</v>
+      </c>
+      <c r="N36" t="s">
+        <v>71</v>
+      </c>
+      <c r="O36" s="2">
+        <v>204809.829</v>
+      </c>
+      <c r="P36" s="1">
+        <v>6.0488405899999996E-4</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <v>34</v>
+      </c>
+      <c r="B37" t="s">
+        <v>50</v>
+      </c>
+      <c r="C37" s="2">
+        <v>10.231609300000001</v>
+      </c>
+      <c r="D37" s="2">
+        <v>1.38054157E-3</v>
+      </c>
+      <c r="E37" s="1">
+        <v>1.01873084E-5</v>
+      </c>
+      <c r="M37">
+        <v>2</v>
+      </c>
+      <c r="N37" t="s">
+        <v>83</v>
+      </c>
+      <c r="O37" s="2">
+        <v>10571150000</v>
+      </c>
+      <c r="P37" s="1">
+        <v>4.2911005400000002E-4</v>
+      </c>
+    </row>
+    <row r="38" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <v>35</v>
+      </c>
+      <c r="B38" t="s">
+        <v>48</v>
+      </c>
+      <c r="C38" s="2">
+        <v>24801.891</v>
+      </c>
+      <c r="D38" s="2">
+        <v>0</v>
+      </c>
+      <c r="E38" s="1">
+        <v>1.11982353E-4</v>
+      </c>
+      <c r="M38">
+        <v>53</v>
+      </c>
+      <c r="N38" t="s">
+        <v>66</v>
+      </c>
+      <c r="O38" s="2">
+        <v>54428.785499999998</v>
+      </c>
+      <c r="P38" s="1">
+        <v>4.2848280399999998E-4</v>
+      </c>
+    </row>
+    <row r="39" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <v>36</v>
+      </c>
+      <c r="B39" t="s">
+        <v>51</v>
+      </c>
+      <c r="C39" s="2">
+        <v>2556.3501099999999</v>
+      </c>
+      <c r="D39" s="2">
+        <v>0</v>
+      </c>
+      <c r="E39" s="1">
+        <v>1.39019085E-4</v>
+      </c>
+      <c r="M39">
+        <v>51</v>
+      </c>
+      <c r="N39" t="s">
+        <v>64</v>
+      </c>
+      <c r="O39" s="2">
+        <v>46699.728900000002</v>
+      </c>
+      <c r="P39" s="1">
+        <v>3.2423230300000002E-4</v>
+      </c>
+    </row>
+    <row r="40" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A40">
+        <v>37</v>
+      </c>
+      <c r="B40" t="s">
+        <v>47</v>
+      </c>
+      <c r="C40" s="2">
+        <v>5859.4743799999997</v>
+      </c>
+      <c r="D40" s="2">
+        <v>0</v>
+      </c>
+      <c r="E40" s="1">
+        <v>1.5653039700000001E-4</v>
+      </c>
+      <c r="M40">
+        <v>27</v>
+      </c>
+      <c r="N40" t="s">
+        <v>32</v>
+      </c>
+      <c r="O40" s="2">
+        <v>2363.9002399999999</v>
+      </c>
+      <c r="P40" s="1">
+        <v>2.67400202E-4</v>
+      </c>
+    </row>
+    <row r="41" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <v>38</v>
+      </c>
+      <c r="B41" t="s">
+        <v>49</v>
+      </c>
+      <c r="C41" s="2">
+        <v>20761.0965</v>
+      </c>
+      <c r="D41" s="2">
+        <v>0</v>
+      </c>
+      <c r="E41" s="1">
+        <v>6.4750826200000002E-4</v>
+      </c>
+      <c r="M41">
+        <v>26</v>
+      </c>
+      <c r="N41" t="s">
+        <v>31</v>
+      </c>
+      <c r="O41" s="2">
+        <v>1723.94676</v>
+      </c>
+      <c r="P41" s="1">
+        <v>1.8261442199999999E-4</v>
+      </c>
+    </row>
+    <row r="42" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A42">
+        <v>39</v>
+      </c>
+      <c r="B42" t="s">
+        <v>52</v>
+      </c>
+      <c r="C42" s="2">
+        <v>154903.18700000001</v>
+      </c>
+      <c r="D42" s="2">
+        <v>0</v>
+      </c>
+      <c r="E42" s="1">
+        <v>1.73985735E-4</v>
+      </c>
+      <c r="M42">
+        <v>39</v>
+      </c>
+      <c r="N42" t="s">
+        <v>52</v>
+      </c>
+      <c r="O42" s="2">
+        <v>154903.18700000001</v>
+      </c>
+      <c r="P42" s="1">
+        <v>1.73985735E-4</v>
+      </c>
+    </row>
+    <row r="43" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A43">
+        <v>40</v>
+      </c>
+      <c r="B43" t="s">
+        <v>53</v>
+      </c>
+      <c r="C43" s="2">
+        <v>87502.690300000002</v>
+      </c>
+      <c r="D43" s="2">
+        <v>0</v>
+      </c>
+      <c r="E43" s="1">
+        <v>3.3587656800000003E-5</v>
+      </c>
+      <c r="M43">
+        <v>0</v>
+      </c>
+      <c r="N43" t="s">
+        <v>81</v>
+      </c>
+      <c r="O43" s="2">
+        <v>145362183000</v>
+      </c>
+      <c r="P43" s="1">
+        <v>1.7028586399999999E-4</v>
+      </c>
+    </row>
+    <row r="44" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A44">
+        <v>41</v>
+      </c>
+      <c r="B44" t="s">
+        <v>57</v>
+      </c>
+      <c r="C44" s="2">
+        <v>13673.6792</v>
+      </c>
+      <c r="D44" s="2">
+        <v>0</v>
+      </c>
+      <c r="E44" s="1">
+        <v>8.1099418100000001E-7</v>
+      </c>
+      <c r="M44">
+        <v>37</v>
+      </c>
+      <c r="N44" t="s">
+        <v>47</v>
+      </c>
+      <c r="O44" s="2">
+        <v>5859.4743799999997</v>
+      </c>
+      <c r="P44" s="1">
+        <v>1.5653039700000001E-4</v>
+      </c>
+    </row>
+    <row r="45" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A45">
+        <v>42</v>
+      </c>
+      <c r="B45" t="s">
+        <v>55</v>
+      </c>
+      <c r="C45" s="2">
+        <v>3661.3737299999998</v>
+      </c>
+      <c r="D45" s="2">
+        <v>0</v>
+      </c>
+      <c r="E45" s="1">
+        <v>1.08791142E-7</v>
+      </c>
+      <c r="M45">
+        <v>50</v>
+      </c>
+      <c r="N45" t="s">
+        <v>63</v>
+      </c>
+      <c r="O45" s="2">
+        <v>27431.142899999999</v>
+      </c>
+      <c r="P45" s="1">
+        <v>1.5587962999999999E-4</v>
+      </c>
+    </row>
+    <row r="46" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A46">
+        <v>43</v>
+      </c>
+      <c r="B46" t="s">
+        <v>54</v>
+      </c>
+      <c r="C46" s="2">
+        <v>2165.8837400000002</v>
+      </c>
+      <c r="D46" s="2">
+        <v>0</v>
+      </c>
+      <c r="E46" s="1">
+        <v>1.80174867E-7</v>
+      </c>
+      <c r="M46">
+        <v>36</v>
+      </c>
+      <c r="N46" t="s">
+        <v>51</v>
+      </c>
+      <c r="O46" s="2">
+        <v>2556.3501099999999</v>
+      </c>
+      <c r="P46" s="1">
+        <v>1.39019085E-4</v>
+      </c>
+    </row>
+    <row r="47" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A47">
+        <v>44</v>
+      </c>
+      <c r="B47" t="s">
+        <v>58</v>
+      </c>
+      <c r="C47" s="2">
+        <v>3161.0840699999999</v>
+      </c>
+      <c r="D47" s="2">
+        <v>0</v>
+      </c>
+      <c r="E47" s="1">
+        <v>1.06180375E-7</v>
+      </c>
+      <c r="M47">
+        <v>1</v>
+      </c>
+      <c r="N47" t="s">
+        <v>82</v>
+      </c>
+      <c r="O47" s="2">
+        <v>135277512000</v>
+      </c>
+      <c r="P47" s="1">
+        <v>1.3878911899999999E-4</v>
+      </c>
+    </row>
+    <row r="48" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A48">
+        <v>45</v>
+      </c>
+      <c r="B48" t="s">
+        <v>56</v>
+      </c>
+      <c r="C48" s="2">
+        <v>10728.320100000001</v>
+      </c>
+      <c r="D48" s="2">
+        <v>0</v>
+      </c>
+      <c r="E48" s="1">
+        <v>1.58350672E-6</v>
+      </c>
+      <c r="M48">
+        <v>35</v>
+      </c>
+      <c r="N48" t="s">
+        <v>48</v>
+      </c>
+      <c r="O48" s="2">
+        <v>24801.891</v>
+      </c>
+      <c r="P48" s="1">
+        <v>1.11982353E-4</v>
+      </c>
+    </row>
+    <row r="49" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A49">
+        <v>46</v>
+      </c>
+      <c r="B49" t="s">
+        <v>59</v>
+      </c>
+      <c r="C49" s="2">
+        <v>633.29216499999995</v>
+      </c>
+      <c r="D49" s="2">
+        <v>9.6118844600000005E-140</v>
+      </c>
+      <c r="E49" s="1">
+        <v>1.3097518200000001E-6</v>
+      </c>
+      <c r="M49">
+        <v>49</v>
+      </c>
+      <c r="N49" t="s">
+        <v>62</v>
+      </c>
+      <c r="O49" s="2">
+        <v>2682.2049999999999</v>
+      </c>
+      <c r="P49" s="1">
+        <v>1.03145398E-4</v>
+      </c>
+    </row>
+    <row r="50" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A50">
+        <v>47</v>
+      </c>
+      <c r="B50" t="s">
+        <v>60</v>
+      </c>
+      <c r="C50" s="2">
+        <v>2907.9465799999998</v>
+      </c>
+      <c r="D50" s="2">
+        <v>0</v>
+      </c>
+      <c r="E50" s="1">
+        <v>5.4834448500000001E-5</v>
+      </c>
+      <c r="M50">
+        <v>14</v>
+      </c>
+      <c r="N50" t="s">
+        <v>95</v>
+      </c>
+      <c r="O50" s="2">
+        <v>7854919520</v>
+      </c>
+      <c r="P50" s="1">
+        <v>8.3318041399999996E-5</v>
+      </c>
+    </row>
+    <row r="51" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A51">
+        <v>48</v>
+      </c>
+      <c r="B51" t="s">
+        <v>61</v>
+      </c>
+      <c r="C51" s="2">
+        <v>8846.4606399999993</v>
+      </c>
+      <c r="D51" s="2">
+        <v>0</v>
+      </c>
+      <c r="E51" s="1">
+        <v>5.9211858700000001E-5</v>
+      </c>
+      <c r="M51">
+        <v>12</v>
+      </c>
+      <c r="N51" t="s">
+        <v>93</v>
+      </c>
+      <c r="O51" s="2">
+        <v>63670269400</v>
+      </c>
+      <c r="P51" s="1">
+        <v>5.9713537299999999E-5</v>
+      </c>
+    </row>
+    <row r="52" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A52">
+        <v>49</v>
+      </c>
+      <c r="B52" t="s">
+        <v>62</v>
+      </c>
+      <c r="C52" s="2">
+        <v>2682.2049999999999</v>
+      </c>
+      <c r="D52" s="2">
+        <v>0</v>
+      </c>
+      <c r="E52" s="1">
+        <v>1.03145398E-4</v>
+      </c>
+      <c r="M52">
+        <v>48</v>
+      </c>
+      <c r="N52" t="s">
+        <v>61</v>
+      </c>
+      <c r="O52" s="2">
+        <v>8846.4606399999993</v>
+      </c>
+      <c r="P52" s="1">
+        <v>5.9211858700000001E-5</v>
+      </c>
+    </row>
+    <row r="53" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A53">
+        <v>50</v>
+      </c>
+      <c r="B53" t="s">
+        <v>63</v>
+      </c>
+      <c r="C53" s="2">
+        <v>27431.142899999999</v>
+      </c>
+      <c r="D53" s="2">
+        <v>0</v>
+      </c>
+      <c r="E53" s="1">
+        <v>1.5587962999999999E-4</v>
+      </c>
+      <c r="M53">
+        <v>47</v>
+      </c>
+      <c r="N53" t="s">
+        <v>60</v>
+      </c>
+      <c r="O53" s="2">
+        <v>2907.9465799999998</v>
+      </c>
+      <c r="P53" s="1">
+        <v>5.4834448500000001E-5</v>
+      </c>
+    </row>
+    <row r="54" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A54">
+        <v>51</v>
+      </c>
+      <c r="B54" t="s">
+        <v>64</v>
+      </c>
+      <c r="C54" s="2">
+        <v>46699.728900000002</v>
+      </c>
+      <c r="D54" s="2">
+        <v>0</v>
+      </c>
+      <c r="E54" s="1">
+        <v>3.2423230300000002E-4</v>
+      </c>
+      <c r="M54">
+        <v>32</v>
+      </c>
+      <c r="N54" t="s">
+        <v>45</v>
+      </c>
+      <c r="O54" s="2">
+        <v>4398.0275300000003</v>
+      </c>
+      <c r="P54" s="1">
+        <v>5.3061747400000002E-5</v>
+      </c>
+    </row>
+    <row r="55" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A55">
+        <v>52</v>
+      </c>
+      <c r="B55" t="s">
+        <v>65</v>
+      </c>
+      <c r="C55" s="2">
+        <v>45201.678099999997</v>
+      </c>
+      <c r="D55" s="2">
+        <v>0</v>
+      </c>
+      <c r="E55" s="1">
+        <v>6.7452916599999998E-4</v>
+      </c>
+      <c r="M55">
+        <v>13</v>
+      </c>
+      <c r="N55" t="s">
+        <v>94</v>
+      </c>
+      <c r="O55" s="2">
+        <v>57198682700</v>
+      </c>
+      <c r="P55" s="1">
+        <v>4.7108162899999998E-5</v>
+      </c>
+    </row>
+    <row r="56" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A56">
+        <v>53</v>
+      </c>
+      <c r="B56" t="s">
+        <v>66</v>
+      </c>
+      <c r="C56" s="2">
+        <v>54428.785499999998</v>
+      </c>
+      <c r="D56" s="2">
+        <v>0</v>
+      </c>
+      <c r="E56" s="1">
+        <v>4.2848280399999998E-4</v>
+      </c>
+      <c r="M56">
+        <v>57</v>
+      </c>
+      <c r="N56" t="s">
+        <v>70</v>
+      </c>
+      <c r="O56" s="2">
+        <v>17604.140100000001</v>
+      </c>
+      <c r="P56" s="1">
+        <v>3.9667279999999997E-5</v>
+      </c>
+    </row>
+    <row r="57" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A57">
+        <v>54</v>
+      </c>
+      <c r="B57" t="s">
+        <v>67</v>
+      </c>
+      <c r="C57" s="2">
+        <v>77053.963600000003</v>
+      </c>
+      <c r="D57" s="2">
+        <v>0</v>
+      </c>
+      <c r="E57" s="1">
+        <v>7.1921307400000004E-4</v>
+      </c>
+      <c r="M57">
+        <v>33</v>
+      </c>
+      <c r="N57" t="s">
+        <v>46</v>
+      </c>
+      <c r="O57" s="2">
+        <v>1399.1057800000001</v>
+      </c>
+      <c r="P57" s="1">
+        <v>3.4387901200000003E-5</v>
+      </c>
+    </row>
+    <row r="58" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A58">
+        <v>55</v>
+      </c>
+      <c r="B58" t="s">
+        <v>68</v>
+      </c>
+      <c r="C58" s="2">
+        <v>68242.3989</v>
+      </c>
+      <c r="D58" s="2">
+        <v>0</v>
+      </c>
+      <c r="E58" s="1">
+        <v>1.5004106200000001E-3</v>
+      </c>
+      <c r="M58">
+        <v>40</v>
+      </c>
+      <c r="N58" t="s">
+        <v>53</v>
+      </c>
+      <c r="O58" s="2">
+        <v>87502.690300000002</v>
+      </c>
+      <c r="P58" s="1">
+        <v>3.3587656800000003E-5</v>
+      </c>
+    </row>
+    <row r="59" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A59">
+        <v>56</v>
+      </c>
+      <c r="B59" t="s">
+        <v>69</v>
+      </c>
+      <c r="C59" s="2">
+        <v>59922.8128</v>
+      </c>
+      <c r="D59" s="2">
+        <v>0</v>
+      </c>
+      <c r="E59" s="1">
+        <v>1.1541742399999999E-3</v>
+      </c>
+      <c r="M59">
+        <v>34</v>
+      </c>
+      <c r="N59" t="s">
+        <v>50</v>
+      </c>
+      <c r="O59" s="2">
+        <v>10.231609300000001</v>
+      </c>
+      <c r="P59" s="1">
+        <v>1.01873084E-5</v>
+      </c>
+    </row>
+    <row r="60" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A60">
+        <v>57</v>
+      </c>
+      <c r="B60" t="s">
+        <v>70</v>
+      </c>
+      <c r="C60" s="2">
+        <v>17604.140100000001</v>
+      </c>
+      <c r="D60" s="2">
+        <v>0</v>
+      </c>
+      <c r="E60" s="1">
+        <v>3.9667279999999997E-5</v>
+      </c>
+      <c r="M60">
+        <v>45</v>
+      </c>
+      <c r="N60" t="s">
+        <v>56</v>
+      </c>
+      <c r="O60" s="2">
+        <v>10728.320100000001</v>
+      </c>
+      <c r="P60" s="1">
+        <v>1.58350672E-6</v>
+      </c>
+    </row>
+    <row r="61" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A61">
+        <v>58</v>
+      </c>
+      <c r="B61" t="s">
+        <v>71</v>
+      </c>
+      <c r="C61" s="2">
+        <v>204809.829</v>
+      </c>
+      <c r="D61" s="2">
+        <v>0</v>
+      </c>
+      <c r="E61" s="1">
+        <v>6.0488405899999996E-4</v>
+      </c>
+      <c r="M61">
+        <v>46</v>
+      </c>
+      <c r="N61" t="s">
+        <v>59</v>
+      </c>
+      <c r="O61" s="2">
+        <v>633.29216499999995</v>
+      </c>
+      <c r="P61" s="1">
+        <v>1.3097518200000001E-6</v>
+      </c>
+    </row>
+    <row r="62" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A62">
+        <v>59</v>
+      </c>
+      <c r="B62" t="s">
+        <v>72</v>
+      </c>
+      <c r="C62" s="2">
+        <v>463414.08100000001</v>
+      </c>
+      <c r="D62" s="2">
+        <v>0</v>
+      </c>
+      <c r="E62" s="1">
+        <v>3.01429916E-3</v>
+      </c>
+      <c r="M62">
+        <v>41</v>
+      </c>
+      <c r="N62" t="s">
+        <v>57</v>
+      </c>
+      <c r="O62" s="2">
+        <v>13673.6792</v>
+      </c>
+      <c r="P62" s="1">
+        <v>8.1099418100000001E-7</v>
+      </c>
+    </row>
+    <row r="63" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A63">
+        <v>60</v>
+      </c>
+      <c r="B63" t="s">
+        <v>73</v>
+      </c>
+      <c r="C63" s="2">
+        <v>476734.81099999999</v>
+      </c>
+      <c r="D63" s="2">
+        <v>0</v>
+      </c>
+      <c r="E63" s="1">
+        <v>4.1012085499999998E-3</v>
+      </c>
+      <c r="M63">
+        <v>43</v>
+      </c>
+      <c r="N63" t="s">
+        <v>54</v>
+      </c>
+      <c r="O63" s="2">
+        <v>2165.8837400000002</v>
+      </c>
+      <c r="P63" s="1">
+        <v>1.80174867E-7</v>
+      </c>
+    </row>
+    <row r="64" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A64">
+        <v>61</v>
+      </c>
+      <c r="B64" t="s">
+        <v>74</v>
+      </c>
+      <c r="C64" s="2">
+        <v>368657.85200000001</v>
+      </c>
+      <c r="D64" s="2">
+        <v>0</v>
+      </c>
+      <c r="E64" s="1">
+        <v>1.63361552E-3</v>
+      </c>
+      <c r="M64">
+        <v>42</v>
+      </c>
+      <c r="N64" t="s">
+        <v>55</v>
+      </c>
+      <c r="O64" s="2">
+        <v>3661.3737299999998</v>
+      </c>
+      <c r="P64" s="1">
+        <v>1.08791142E-7</v>
+      </c>
+    </row>
+    <row r="65" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A65">
+        <v>62</v>
+      </c>
+      <c r="B65" t="s">
+        <v>75</v>
+      </c>
+      <c r="C65" s="2">
+        <v>233485.66800000001</v>
+      </c>
+      <c r="D65" s="2">
+        <v>0</v>
+      </c>
+      <c r="E65" s="1">
+        <v>6.3247038699999997E-4</v>
+      </c>
+      <c r="M65">
+        <v>44</v>
+      </c>
+      <c r="N65" t="s">
+        <v>58</v>
+      </c>
+      <c r="O65" s="2">
+        <v>3161.0840699999999</v>
+      </c>
+      <c r="P65" s="1">
+        <v>1.06180375E-7</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState ref="M3:P65">
+    <sortCondition descending="1" ref="P3"/>
+  </sortState>
+  <conditionalFormatting sqref="P3:P65">
+    <cfRule type="dataBar" priority="1">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF638EC6"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{6CAFAC52-B447-429C-AF4F-8FEE74D2109E}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
+      <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{6CAFAC52-B447-429C-AF4F-8FEE74D2109E}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FF638EC6"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>P3:P65</xm:sqref>
+        </x14:conditionalFormatting>
+      </x14:conditionalFormattings>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
modified codes to make the pipeline more coherent, added code to include all targets while training
</commit_message>
<xml_diff>
--- a/hackerearth_ml3_adclick/analysis_graphs/feature_selection.xlsx
+++ b/hackerearth_ml3_adclick/analysis_graphs/feature_selection.xlsx
@@ -9,12 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="7200" yWindow="0" windowWidth="22104" windowHeight="11016" activeTab="2"/>
+    <workbookView xWindow="8088" yWindow="0" windowWidth="22104" windowHeight="11016" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="137">
   <si>
     <t>chi square values</t>
   </si>
@@ -317,6 +318,126 @@
   </si>
   <si>
     <t>click_rate_category</t>
+  </si>
+  <si>
+    <t>merchant_count</t>
+  </si>
+  <si>
+    <t>merchant_num_0</t>
+  </si>
+  <si>
+    <t>merchant_num_1</t>
+  </si>
+  <si>
+    <t>merchant_click_rate</t>
+  </si>
+  <si>
+    <t>siteid_count</t>
+  </si>
+  <si>
+    <t>siteid_num_0</t>
+  </si>
+  <si>
+    <t>siteid_num_1</t>
+  </si>
+  <si>
+    <t>siteid_click_rate</t>
+  </si>
+  <si>
+    <t>offerid_count</t>
+  </si>
+  <si>
+    <t>offerid_num_0</t>
+  </si>
+  <si>
+    <t>offerid_num_1</t>
+  </si>
+  <si>
+    <t>offerid_click_rate</t>
+  </si>
+  <si>
+    <t>category_count</t>
+  </si>
+  <si>
+    <t>category_num_0</t>
+  </si>
+  <si>
+    <t>category_num_1</t>
+  </si>
+  <si>
+    <t>category_click_rate</t>
+  </si>
+  <si>
+    <t>countrycode_count</t>
+  </si>
+  <si>
+    <t>countrycode_num_0</t>
+  </si>
+  <si>
+    <t>countrycode_num_1</t>
+  </si>
+  <si>
+    <t>countrycode_click_rate</t>
+  </si>
+  <si>
+    <t>browserid_count</t>
+  </si>
+  <si>
+    <t>browserid_num_0</t>
+  </si>
+  <si>
+    <t>browserid_num_1</t>
+  </si>
+  <si>
+    <t>browserid_click_rate</t>
+  </si>
+  <si>
+    <t>devid_count</t>
+  </si>
+  <si>
+    <t>devid_num_0</t>
+  </si>
+  <si>
+    <t>devid_num_1</t>
+  </si>
+  <si>
+    <t>devid_click_rate</t>
+  </si>
+  <si>
+    <t>datetime_hour_count</t>
+  </si>
+  <si>
+    <t>datetime_hour_num_0</t>
+  </si>
+  <si>
+    <t>datetime_hour_num_1</t>
+  </si>
+  <si>
+    <t>datetime_hour_click_rate</t>
+  </si>
+  <si>
+    <t>datetime_day_count</t>
+  </si>
+  <si>
+    <t>datetime_day_num_0</t>
+  </si>
+  <si>
+    <t>datetime_day_num_1</t>
+  </si>
+  <si>
+    <t>datetime_day_click_rate</t>
+  </si>
+  <si>
+    <t>datetime_minute_count</t>
+  </si>
+  <si>
+    <t>datetime_minute_num_0</t>
+  </si>
+  <si>
+    <t>datetime_minute_num_1</t>
+  </si>
+  <si>
+    <t>datetime_minute_click_rate</t>
   </si>
 </sst>
 </file>
@@ -5909,7 +6030,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+    <sheetView topLeftCell="F1" workbookViewId="0">
       <selection activeCell="N13" sqref="N13"/>
     </sheetView>
   </sheetViews>
@@ -7847,4 +7968,2878 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A4:F156"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="24.21875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>18</v>
+      </c>
+      <c r="B4" t="s">
+        <v>115</v>
+      </c>
+      <c r="C4" s="1">
+        <v>0.13857545099999999</v>
+      </c>
+      <c r="D4" s="1">
+        <v>0.137817891</v>
+      </c>
+      <c r="E4" s="1">
+        <v>0.13837664899999999</v>
+      </c>
+      <c r="F4" s="1">
+        <v>0.136643864</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>17</v>
+      </c>
+      <c r="B5" t="s">
+        <v>114</v>
+      </c>
+      <c r="C5" s="1">
+        <v>9.4179317799999995E-2</v>
+      </c>
+      <c r="D5" s="1">
+        <v>9.69719109E-2</v>
+      </c>
+      <c r="E5" s="1">
+        <v>9.1794301800000005E-2</v>
+      </c>
+      <c r="F5" s="1">
+        <v>9.2464864800000005E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>16</v>
+      </c>
+      <c r="B6" t="s">
+        <v>113</v>
+      </c>
+      <c r="C6" s="1">
+        <v>8.4554843500000004E-2</v>
+      </c>
+      <c r="D6" s="1">
+        <v>8.1541757300000003E-2</v>
+      </c>
+      <c r="E6" s="1">
+        <v>7.9326784900000002E-2</v>
+      </c>
+      <c r="F6" s="1">
+        <v>7.7064055399999998E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>19</v>
+      </c>
+      <c r="B7" t="s">
+        <v>116</v>
+      </c>
+      <c r="C7" s="1">
+        <v>8.1426050900000005E-2</v>
+      </c>
+      <c r="D7" s="1">
+        <v>8.1051085100000003E-2</v>
+      </c>
+      <c r="E7" s="1">
+        <v>8.2554350900000004E-2</v>
+      </c>
+      <c r="F7" s="1">
+        <v>8.8291209300000006E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>20</v>
+      </c>
+      <c r="B8" t="s">
+        <v>117</v>
+      </c>
+      <c r="C8" s="1">
+        <v>7.4245010599999994E-2</v>
+      </c>
+      <c r="D8" s="1">
+        <v>6.4274323800000005E-2</v>
+      </c>
+      <c r="E8" s="1">
+        <v>7.1194194399999994E-2</v>
+      </c>
+      <c r="F8" s="1">
+        <v>7.5079513799999997E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>22</v>
+      </c>
+      <c r="B9" t="s">
+        <v>119</v>
+      </c>
+      <c r="C9" s="1">
+        <v>7.1116830300000003E-2</v>
+      </c>
+      <c r="D9" s="1">
+        <v>7.4895667200000002E-2</v>
+      </c>
+      <c r="E9" s="1">
+        <v>7.2270792599999994E-2</v>
+      </c>
+      <c r="F9" s="1">
+        <v>7.0892104999999997E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>21</v>
+      </c>
+      <c r="B10" t="s">
+        <v>118</v>
+      </c>
+      <c r="C10" s="1">
+        <v>6.0588619099999998E-2</v>
+      </c>
+      <c r="D10" s="1">
+        <v>5.9959424900000002E-2</v>
+      </c>
+      <c r="E10" s="1">
+        <v>6.0842321800000002E-2</v>
+      </c>
+      <c r="F10" s="1">
+        <v>6.1886509499999999E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>23</v>
+      </c>
+      <c r="B11" t="s">
+        <v>120</v>
+      </c>
+      <c r="C11" s="1">
+        <v>5.2766930599999998E-2</v>
+      </c>
+      <c r="D11" s="1">
+        <v>5.5973316500000002E-2</v>
+      </c>
+      <c r="E11" s="1">
+        <v>5.5356923799999999E-2</v>
+      </c>
+      <c r="F11" s="1">
+        <v>5.3510185000000002E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>108</v>
+      </c>
+      <c r="C12" s="1">
+        <v>5.1029870300000002E-2</v>
+      </c>
+      <c r="D12" s="1">
+        <v>5.2608720400000003E-2</v>
+      </c>
+      <c r="E12" s="1">
+        <v>5.3887719799999997E-2</v>
+      </c>
+      <c r="F12" s="1">
+        <v>4.9964704899999997E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>10</v>
+      </c>
+      <c r="B13" t="s">
+        <v>107</v>
+      </c>
+      <c r="C13" s="1">
+        <v>3.9498053700000001E-2</v>
+      </c>
+      <c r="D13" s="1">
+        <v>4.1023798E-2</v>
+      </c>
+      <c r="E13" s="1">
+        <v>3.9299039199999997E-2</v>
+      </c>
+      <c r="F13" s="1">
+        <v>3.91608175E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>7</v>
+      </c>
+      <c r="B14" t="s">
+        <v>104</v>
+      </c>
+      <c r="C14" s="1">
+        <v>3.7496306100000001E-2</v>
+      </c>
+      <c r="D14" s="1">
+        <v>3.74969754E-2</v>
+      </c>
+      <c r="E14" s="1">
+        <v>4.0607043199999998E-2</v>
+      </c>
+      <c r="F14" s="1">
+        <v>3.7957578499999999E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>6</v>
+      </c>
+      <c r="B15" t="s">
+        <v>103</v>
+      </c>
+      <c r="C15" s="1">
+        <v>3.4849246299999997E-2</v>
+      </c>
+      <c r="D15" s="1">
+        <v>3.54086204E-2</v>
+      </c>
+      <c r="E15" s="1">
+        <v>3.6099256000000003E-2</v>
+      </c>
+      <c r="F15" s="1">
+        <v>3.6731602299999999E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>5</v>
+      </c>
+      <c r="B16" t="s">
+        <v>102</v>
+      </c>
+      <c r="C16" s="1">
+        <v>3.1728669600000002E-2</v>
+      </c>
+      <c r="D16" s="1">
+        <v>3.3815867999999999E-2</v>
+      </c>
+      <c r="E16" s="1">
+        <v>3.4332309800000002E-2</v>
+      </c>
+      <c r="F16" s="1">
+        <v>3.4400486799999998E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>4</v>
+      </c>
+      <c r="B17" t="s">
+        <v>101</v>
+      </c>
+      <c r="C17" s="1">
+        <v>2.0324874600000001E-2</v>
+      </c>
+      <c r="D17" s="1">
+        <v>1.87055351E-2</v>
+      </c>
+      <c r="E17" s="1">
+        <v>1.9062549500000001E-2</v>
+      </c>
+      <c r="F17" s="1">
+        <v>1.9784855300000001E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>53</v>
+      </c>
+      <c r="C18" s="1">
+        <v>1.5871888800000001E-2</v>
+      </c>
+      <c r="D18" s="1">
+        <v>1.5951697099999999E-2</v>
+      </c>
+      <c r="E18" s="1">
+        <v>1.43467639E-2</v>
+      </c>
+      <c r="F18" s="1">
+        <v>1.5950260500000001E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>41</v>
+      </c>
+      <c r="B19" t="s">
+        <v>16</v>
+      </c>
+      <c r="C19" s="1">
+        <v>1.3857426000000001E-2</v>
+      </c>
+      <c r="D19" s="1">
+        <v>1.42526054E-2</v>
+      </c>
+      <c r="E19" s="1">
+        <v>1.43342088E-2</v>
+      </c>
+      <c r="F19" s="1">
+        <v>1.29356829E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>42</v>
+      </c>
+      <c r="B20" t="s">
+        <v>17</v>
+      </c>
+      <c r="C20" s="1">
+        <v>1.1632463399999999E-2</v>
+      </c>
+      <c r="D20" s="1">
+        <v>1.1970622199999999E-2</v>
+      </c>
+      <c r="E20" s="1">
+        <v>1.12063049E-2</v>
+      </c>
+      <c r="F20" s="1">
+        <v>1.0993569999999999E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>48</v>
+      </c>
+      <c r="C21" s="1">
+        <v>1.1070010599999999E-2</v>
+      </c>
+      <c r="D21" s="1">
+        <v>1.0801379700000001E-2</v>
+      </c>
+      <c r="E21" s="1">
+        <v>1.2003720000000001E-2</v>
+      </c>
+      <c r="F21" s="1">
+        <v>1.1010228299999999E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>26</v>
+      </c>
+      <c r="B22" t="s">
+        <v>123</v>
+      </c>
+      <c r="C22" s="1">
+        <v>1.0184099300000001E-2</v>
+      </c>
+      <c r="D22" s="1">
+        <v>1.0124619499999999E-2</v>
+      </c>
+      <c r="E22" s="1">
+        <v>1.01143945E-2</v>
+      </c>
+      <c r="F22" s="1">
+        <v>1.0268122100000001E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>50</v>
+      </c>
+      <c r="C23" s="1">
+        <v>8.1926361800000007E-3</v>
+      </c>
+      <c r="D23" s="1">
+        <v>8.0834528300000007E-3</v>
+      </c>
+      <c r="E23" s="1">
+        <v>7.6384153600000003E-3</v>
+      </c>
+      <c r="F23" s="1">
+        <v>7.9308439399999996E-3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>49</v>
+      </c>
+      <c r="C24" s="1">
+        <v>7.37161125E-3</v>
+      </c>
+      <c r="D24" s="1">
+        <v>7.4282625600000001E-3</v>
+      </c>
+      <c r="E24" s="1">
+        <v>7.4807694100000001E-3</v>
+      </c>
+      <c r="F24" s="1">
+        <v>7.1600945500000001E-3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>61</v>
+      </c>
+      <c r="C25" s="1">
+        <v>5.8110497100000002E-3</v>
+      </c>
+      <c r="D25" s="1">
+        <v>5.58209967E-3</v>
+      </c>
+      <c r="E25" s="1">
+        <v>5.0574492400000002E-3</v>
+      </c>
+      <c r="F25" s="1">
+        <v>5.6679075600000002E-3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>31</v>
+      </c>
+      <c r="B26" t="s">
+        <v>128</v>
+      </c>
+      <c r="C26" s="1">
+        <v>5.6133064600000001E-3</v>
+      </c>
+      <c r="D26" s="1">
+        <v>5.7544433300000001E-3</v>
+      </c>
+      <c r="E26" s="1">
+        <v>5.95162204E-3</v>
+      </c>
+      <c r="F26" s="1">
+        <v>6.3527681100000004E-3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>29</v>
+      </c>
+      <c r="B27" t="s">
+        <v>126</v>
+      </c>
+      <c r="C27" s="1">
+        <v>5.03460808E-3</v>
+      </c>
+      <c r="D27" s="1">
+        <v>5.8857754600000001E-3</v>
+      </c>
+      <c r="E27" s="1">
+        <v>5.22397231E-3</v>
+      </c>
+      <c r="F27" s="1">
+        <v>5.21601567E-3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>40</v>
+      </c>
+      <c r="B28" t="s">
+        <v>15</v>
+      </c>
+      <c r="C28" s="1">
+        <v>4.5888930499999999E-3</v>
+      </c>
+      <c r="D28" s="1">
+        <v>4.65437861E-3</v>
+      </c>
+      <c r="E28" s="1">
+        <v>4.1118506300000003E-3</v>
+      </c>
+      <c r="F28" s="1">
+        <v>4.82845601E-3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29" t="s">
+        <v>125</v>
+      </c>
+      <c r="C29" s="1">
+        <v>4.4863104600000002E-3</v>
+      </c>
+      <c r="D29" s="1">
+        <v>4.0819551300000003E-3</v>
+      </c>
+      <c r="E29" s="1">
+        <v>4.4133208600000001E-3</v>
+      </c>
+      <c r="F29" s="1">
+        <v>4.8811835200000004E-3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>27</v>
+      </c>
+      <c r="B30" t="s">
+        <v>124</v>
+      </c>
+      <c r="C30" s="1">
+        <v>2.9175726600000002E-3</v>
+      </c>
+      <c r="D30" s="1">
+        <v>1.88759107E-3</v>
+      </c>
+      <c r="E30" s="1">
+        <v>1.6334829800000001E-3</v>
+      </c>
+      <c r="F30" s="1">
+        <v>2.3117620899999998E-3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>43</v>
+      </c>
+      <c r="B31" t="s">
+        <v>18</v>
+      </c>
+      <c r="C31" s="1">
+        <v>2.7334546500000002E-3</v>
+      </c>
+      <c r="D31" s="1">
+        <v>2.8589304699999998E-3</v>
+      </c>
+      <c r="E31" s="1">
+        <v>2.8792901000000001E-3</v>
+      </c>
+      <c r="F31" s="1">
+        <v>2.8075788900000002E-3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>25</v>
+      </c>
+      <c r="B32" t="s">
+        <v>122</v>
+      </c>
+      <c r="C32" s="1">
+        <v>2.23311465E-3</v>
+      </c>
+      <c r="D32" s="1">
+        <v>2.2454484099999998E-3</v>
+      </c>
+      <c r="E32" s="1">
+        <v>2.1014015400000001E-3</v>
+      </c>
+      <c r="F32" s="1">
+        <v>2.1611555300000002E-3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>3</v>
+      </c>
+      <c r="B33" t="s">
+        <v>100</v>
+      </c>
+      <c r="C33" s="1">
+        <v>1.97256964E-3</v>
+      </c>
+      <c r="D33" s="1">
+        <v>1.9191123799999999E-3</v>
+      </c>
+      <c r="E33" s="1">
+        <v>2.3523980500000001E-3</v>
+      </c>
+      <c r="F33" s="1">
+        <v>1.2910134000000001E-3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <v>24</v>
+      </c>
+      <c r="B34" t="s">
+        <v>121</v>
+      </c>
+      <c r="C34" s="1">
+        <v>1.8835266200000001E-3</v>
+      </c>
+      <c r="D34" s="1">
+        <v>2.2653170899999998E-3</v>
+      </c>
+      <c r="E34" s="1">
+        <v>1.9975926800000002E-3</v>
+      </c>
+      <c r="F34" s="1">
+        <v>1.90132353E-3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <v>9</v>
+      </c>
+      <c r="B35" t="s">
+        <v>106</v>
+      </c>
+      <c r="C35" s="1">
+        <v>1.68745154E-3</v>
+      </c>
+      <c r="D35" s="1">
+        <v>1.7085347399999999E-3</v>
+      </c>
+      <c r="E35" s="1">
+        <v>1.64889218E-3</v>
+      </c>
+      <c r="F35" s="1">
+        <v>1.67366271E-3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <v>30</v>
+      </c>
+      <c r="B36" t="s">
+        <v>127</v>
+      </c>
+      <c r="C36" s="1">
+        <v>1.6782347500000001E-3</v>
+      </c>
+      <c r="D36" s="1">
+        <v>2.0783269900000001E-3</v>
+      </c>
+      <c r="E36" s="1">
+        <v>1.59487608E-3</v>
+      </c>
+      <c r="F36" s="1">
+        <v>1.2045863199999999E-3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <v>54</v>
+      </c>
+      <c r="C37" s="1">
+        <v>1.5665286300000001E-3</v>
+      </c>
+      <c r="D37" s="1">
+        <v>1.4734483599999999E-3</v>
+      </c>
+      <c r="E37" s="1">
+        <v>1.6061068900000001E-3</v>
+      </c>
+      <c r="F37" s="1">
+        <v>1.4295055100000001E-3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <v>60</v>
+      </c>
+      <c r="C38" s="1">
+        <v>1.02936949E-3</v>
+      </c>
+      <c r="D38" s="1">
+        <v>1.0567078499999999E-3</v>
+      </c>
+      <c r="E38" s="1">
+        <v>1.0528894499999999E-3</v>
+      </c>
+      <c r="F38" s="1">
+        <v>1.0422676100000001E-3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <v>55</v>
+      </c>
+      <c r="C39" s="1">
+        <v>9.8635237700000003E-4</v>
+      </c>
+      <c r="D39" s="1">
+        <v>9.5229096799999999E-4</v>
+      </c>
+      <c r="E39" s="1">
+        <v>1.0224577600000001E-3</v>
+      </c>
+      <c r="F39" s="1">
+        <v>9.2718993899999996E-4</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A40">
+        <v>15</v>
+      </c>
+      <c r="B40" t="s">
+        <v>112</v>
+      </c>
+      <c r="C40" s="1">
+        <v>6.9653295200000002E-4</v>
+      </c>
+      <c r="D40" s="1">
+        <v>7.4160222400000003E-4</v>
+      </c>
+      <c r="E40" s="1">
+        <v>7.7998857599999999E-4</v>
+      </c>
+      <c r="F40" s="1">
+        <v>8.4494143799999997E-4</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <v>90</v>
+      </c>
+      <c r="C41" s="1">
+        <v>6.4668872400000001E-4</v>
+      </c>
+      <c r="D41" s="1">
+        <v>5.9314775399999995E-4</v>
+      </c>
+      <c r="E41" s="1">
+        <v>5.3810240800000004E-4</v>
+      </c>
+      <c r="F41" s="1">
+        <v>6.2213484299999998E-4</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A42">
+        <v>2</v>
+      </c>
+      <c r="B42" t="s">
+        <v>99</v>
+      </c>
+      <c r="C42" s="1">
+        <v>4.7768864500000001E-4</v>
+      </c>
+      <c r="D42" s="1">
+        <v>3.9052849900000002E-4</v>
+      </c>
+      <c r="E42" s="1">
+        <v>4.6052643599999999E-4</v>
+      </c>
+      <c r="F42" s="1">
+        <v>4.9369687800000003E-4</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A43">
+        <v>8</v>
+      </c>
+      <c r="B43" t="s">
+        <v>105</v>
+      </c>
+      <c r="C43" s="1">
+        <v>3.4512212999999998E-4</v>
+      </c>
+      <c r="D43" s="1">
+        <v>4.01602076E-4</v>
+      </c>
+      <c r="E43" s="1">
+        <v>3.17806966E-4</v>
+      </c>
+      <c r="F43" s="1">
+        <v>3.9623890899999998E-4</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A44">
+        <v>46</v>
+      </c>
+      <c r="C44" s="1">
+        <v>3.1805075099999999E-4</v>
+      </c>
+      <c r="D44" s="1">
+        <v>3.1454524200000001E-4</v>
+      </c>
+      <c r="E44" s="1">
+        <v>2.99520491E-4</v>
+      </c>
+      <c r="F44" s="1">
+        <v>3.7115123799999998E-4</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A45">
+        <v>89</v>
+      </c>
+      <c r="C45" s="1">
+        <v>2.9658242600000002E-4</v>
+      </c>
+      <c r="D45" s="1">
+        <v>2.25946768E-4</v>
+      </c>
+      <c r="E45" s="1">
+        <v>2.9887161600000001E-4</v>
+      </c>
+      <c r="F45" s="1">
+        <v>2.7398815599999999E-4</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A46">
+        <v>45</v>
+      </c>
+      <c r="B46" t="s">
+        <v>20</v>
+      </c>
+      <c r="C46" s="1">
+        <v>2.62784519E-4</v>
+      </c>
+      <c r="D46" s="1">
+        <v>3.96367571E-4</v>
+      </c>
+      <c r="E46" s="1">
+        <v>3.3312430799999998E-4</v>
+      </c>
+      <c r="F46" s="1">
+        <v>3.1570191299999998E-4</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A47">
+        <v>59</v>
+      </c>
+      <c r="C47" s="1">
+        <v>2.4186845400000001E-4</v>
+      </c>
+      <c r="D47" s="1">
+        <v>3.00711923E-4</v>
+      </c>
+      <c r="E47" s="1">
+        <v>2.4128263299999999E-4</v>
+      </c>
+      <c r="F47" s="1">
+        <v>7.5213491600000003E-4</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A48">
+        <v>14</v>
+      </c>
+      <c r="B48" t="s">
+        <v>111</v>
+      </c>
+      <c r="C48" s="1">
+        <v>2.2592694500000001E-4</v>
+      </c>
+      <c r="D48" s="1">
+        <v>2.4621870199999999E-4</v>
+      </c>
+      <c r="E48" s="1">
+        <v>2.4109451599999999E-4</v>
+      </c>
+      <c r="F48" s="1">
+        <v>2.6215164900000003E-4</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A49">
+        <v>13</v>
+      </c>
+      <c r="B49" t="s">
+        <v>110</v>
+      </c>
+      <c r="C49" s="1">
+        <v>2.0926522799999999E-4</v>
+      </c>
+      <c r="D49" s="1">
+        <v>2.6262860400000002E-4</v>
+      </c>
+      <c r="E49" s="1">
+        <v>2.0051150700000001E-4</v>
+      </c>
+      <c r="F49" s="1">
+        <v>9.5148321100000001E-5</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A50">
+        <v>91</v>
+      </c>
+      <c r="C50" s="1">
+        <v>1.92412539E-4</v>
+      </c>
+      <c r="D50" s="1">
+        <v>1.5778809000000001E-4</v>
+      </c>
+      <c r="E50" s="1">
+        <v>2.3195524499999999E-4</v>
+      </c>
+      <c r="F50" s="1">
+        <v>2.31818044E-4</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A51">
+        <v>44</v>
+      </c>
+      <c r="B51" t="s">
+        <v>19</v>
+      </c>
+      <c r="C51" s="1">
+        <v>1.87642282E-4</v>
+      </c>
+      <c r="D51" s="1">
+        <v>2.27554314E-4</v>
+      </c>
+      <c r="E51" s="1">
+        <v>2.37502253E-4</v>
+      </c>
+      <c r="F51" s="1">
+        <v>2.7535590699999998E-4</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A52">
+        <v>47</v>
+      </c>
+      <c r="C52" s="1">
+        <v>1.8031587E-4</v>
+      </c>
+      <c r="D52" s="1">
+        <v>1.9287329699999999E-4</v>
+      </c>
+      <c r="E52" s="1">
+        <v>1.7748630099999999E-4</v>
+      </c>
+      <c r="F52" s="1">
+        <v>1.7058291600000001E-4</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A53">
+        <v>51</v>
+      </c>
+      <c r="C53" s="1">
+        <v>1.8007035200000001E-4</v>
+      </c>
+      <c r="D53" s="1">
+        <v>1.9979022099999999E-4</v>
+      </c>
+      <c r="E53" s="1">
+        <v>1.2777016900000001E-4</v>
+      </c>
+      <c r="F53" s="1">
+        <v>1.72902496E-4</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A54">
+        <v>92</v>
+      </c>
+      <c r="C54" s="1">
+        <v>1.3081604599999999E-4</v>
+      </c>
+      <c r="D54" s="1">
+        <v>1.2876914899999999E-4</v>
+      </c>
+      <c r="E54" s="1">
+        <v>1.1885057199999999E-4</v>
+      </c>
+      <c r="F54" s="1">
+        <v>1.26990949E-4</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A55">
+        <v>88</v>
+      </c>
+      <c r="C55" s="1">
+        <v>1.26524871E-4</v>
+      </c>
+      <c r="D55" s="1">
+        <v>1.33922236E-4</v>
+      </c>
+      <c r="E55" s="1">
+        <v>1.5636700500000001E-4</v>
+      </c>
+      <c r="F55" s="1">
+        <v>2.4665995500000002E-4</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A56">
+        <v>52</v>
+      </c>
+      <c r="C56" s="1">
+        <v>1.23719428E-4</v>
+      </c>
+      <c r="D56" s="1">
+        <v>1.3356459099999999E-4</v>
+      </c>
+      <c r="E56" s="1">
+        <v>3.4445765099999997E-5</v>
+      </c>
+      <c r="F56" s="1">
+        <v>1.81329729E-4</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A57">
+        <v>12</v>
+      </c>
+      <c r="B57" t="s">
+        <v>109</v>
+      </c>
+      <c r="C57" s="1">
+        <v>1.1146524400000001E-4</v>
+      </c>
+      <c r="D57" s="1">
+        <v>8.0525386400000001E-5</v>
+      </c>
+      <c r="E57" s="1">
+        <v>6.0320536100000003E-5</v>
+      </c>
+      <c r="F57" s="1">
+        <v>7.4260224400000003E-5</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A58">
+        <v>70</v>
+      </c>
+      <c r="C58" s="1">
+        <v>6.57352085E-5</v>
+      </c>
+      <c r="D58" s="1">
+        <v>6.16602469E-5</v>
+      </c>
+      <c r="E58" s="1">
+        <v>6.6923086000000005E-5</v>
+      </c>
+      <c r="F58" s="1">
+        <v>6.25642992E-5</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A59">
+        <v>57</v>
+      </c>
+      <c r="C59" s="1">
+        <v>3.4311920499999999E-5</v>
+      </c>
+      <c r="D59" s="1">
+        <v>8.23994403E-5</v>
+      </c>
+      <c r="E59" s="1">
+        <v>4.8650073800000003E-5</v>
+      </c>
+      <c r="F59" s="1">
+        <v>3.6239834399999998E-5</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A60">
+        <v>0</v>
+      </c>
+      <c r="B60" t="s">
+        <v>97</v>
+      </c>
+      <c r="C60" s="1">
+        <v>3.2199369100000002E-5</v>
+      </c>
+      <c r="D60" s="1">
+        <v>3.8551255000000002E-5</v>
+      </c>
+      <c r="E60" s="1">
+        <v>2.61499926E-5</v>
+      </c>
+      <c r="F60" s="1">
+        <v>3.2639578799999998E-5</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A61">
+        <v>69</v>
+      </c>
+      <c r="C61" s="1">
+        <v>2.86079412E-5</v>
+      </c>
+      <c r="D61" s="1">
+        <v>9.4284643699999997E-6</v>
+      </c>
+      <c r="E61" s="1">
+        <v>9.8278546100000002E-5</v>
+      </c>
+      <c r="F61" s="1">
+        <v>1.4478591600000001E-5</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A62">
+        <v>1</v>
+      </c>
+      <c r="B62" t="s">
+        <v>98</v>
+      </c>
+      <c r="C62" s="1">
+        <v>2.4769440500000001E-5</v>
+      </c>
+      <c r="D62" s="1">
+        <v>2.02820025E-5</v>
+      </c>
+      <c r="E62" s="1">
+        <v>2.3922953399999999E-5</v>
+      </c>
+      <c r="F62" s="1">
+        <v>3.2369105999999998E-5</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A63">
+        <v>34</v>
+      </c>
+      <c r="B63" t="s">
+        <v>131</v>
+      </c>
+      <c r="C63" s="1">
+        <v>2.07838146E-5</v>
+      </c>
+      <c r="D63" s="1">
+        <v>2.3824622100000001E-5</v>
+      </c>
+      <c r="E63" s="1">
+        <v>2.9507410399999999E-5</v>
+      </c>
+      <c r="F63" s="1">
+        <v>1.7485186600000001E-5</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A64">
+        <v>84</v>
+      </c>
+      <c r="C64" s="1">
+        <v>1.1518366E-5</v>
+      </c>
+      <c r="D64" s="1">
+        <v>1.1657208199999999E-5</v>
+      </c>
+      <c r="E64" s="1">
+        <v>1.1324757600000001E-5</v>
+      </c>
+      <c r="F64" s="1">
+        <v>1.12208523E-5</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A65">
+        <v>81</v>
+      </c>
+      <c r="C65" s="1">
+        <v>6.4486406699999999E-6</v>
+      </c>
+      <c r="D65" s="1">
+        <v>2.2158605700000002E-6</v>
+      </c>
+      <c r="E65" s="1">
+        <v>5.3801007400000001E-6</v>
+      </c>
+      <c r="F65" s="1">
+        <v>1.9948435000000002E-6</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A66">
+        <v>33</v>
+      </c>
+      <c r="B66" t="s">
+        <v>130</v>
+      </c>
+      <c r="C66" s="1">
+        <v>6.0834059999999998E-6</v>
+      </c>
+      <c r="D66" s="1">
+        <v>6.0754387899999998E-6</v>
+      </c>
+      <c r="E66" s="1">
+        <v>8.3106504099999994E-6</v>
+      </c>
+      <c r="F66" s="1">
+        <v>2.5452727200000002E-6</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A67">
+        <v>35</v>
+      </c>
+      <c r="B67" t="s">
+        <v>132</v>
+      </c>
+      <c r="C67" s="1">
+        <v>4.7954663900000003E-6</v>
+      </c>
+      <c r="D67" s="1">
+        <v>1.31976895E-5</v>
+      </c>
+      <c r="E67" s="1">
+        <v>6.1466322899999998E-6</v>
+      </c>
+      <c r="F67" s="1">
+        <v>8.1549314099999999E-6</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A68">
+        <v>85</v>
+      </c>
+      <c r="C68" s="1">
+        <v>4.7024001900000001E-6</v>
+      </c>
+      <c r="D68" s="1">
+        <v>4.1825248899999996E-6</v>
+      </c>
+      <c r="E68" s="1">
+        <v>1.2799628499999999E-6</v>
+      </c>
+      <c r="F68" s="1">
+        <v>5.9492494199999998E-6</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A69">
+        <v>32</v>
+      </c>
+      <c r="B69" t="s">
+        <v>129</v>
+      </c>
+      <c r="C69" s="1">
+        <v>4.0761647399999996E-6</v>
+      </c>
+      <c r="D69" s="1">
+        <v>3.9011785899999996E-6</v>
+      </c>
+      <c r="E69" s="1">
+        <v>3.5087242099999999E-6</v>
+      </c>
+      <c r="F69" s="1">
+        <v>8.2362118399999998E-6</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A70">
+        <v>65</v>
+      </c>
+      <c r="C70" s="1">
+        <v>3.2554783200000001E-6</v>
+      </c>
+      <c r="D70" s="1">
+        <v>2.7636499300000002E-6</v>
+      </c>
+      <c r="E70" s="1">
+        <v>3.13325437E-6</v>
+      </c>
+      <c r="F70" s="1">
+        <v>3.0605750100000002E-6</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A71">
+        <v>82</v>
+      </c>
+      <c r="C71" s="1">
+        <v>3.15016078E-6</v>
+      </c>
+      <c r="D71" s="1">
+        <v>2.43784372E-6</v>
+      </c>
+      <c r="E71" s="1">
+        <v>1.82853784E-6</v>
+      </c>
+      <c r="F71" s="1">
+        <v>4.37705284E-6</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A72">
+        <v>39</v>
+      </c>
+      <c r="B72" t="s">
+        <v>136</v>
+      </c>
+      <c r="C72" s="1">
+        <v>2.9753315200000001E-6</v>
+      </c>
+      <c r="D72" s="1">
+        <v>1.9530850399999999E-6</v>
+      </c>
+      <c r="E72" s="1">
+        <v>1.9042924600000001E-6</v>
+      </c>
+      <c r="F72" s="1">
+        <v>3.5452843E-6</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A73">
+        <v>68</v>
+      </c>
+      <c r="C73" s="1">
+        <v>1.8367258599999999E-6</v>
+      </c>
+      <c r="D73" s="1">
+        <v>9.3729425500000003E-7</v>
+      </c>
+      <c r="E73" s="1">
+        <v>1.3364843100000001E-6</v>
+      </c>
+      <c r="F73" s="1">
+        <v>2.6572867999999999E-6</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A74">
+        <v>108</v>
+      </c>
+      <c r="C74" s="1">
+        <v>9.1086372300000005E-7</v>
+      </c>
+      <c r="D74" s="1">
+        <v>2.6934915399999998E-9</v>
+      </c>
+      <c r="E74" s="1">
+        <v>0</v>
+      </c>
+      <c r="F74" s="1">
+        <v>2.5420106199999997E-7</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A75">
+        <v>37</v>
+      </c>
+      <c r="B75" t="s">
+        <v>134</v>
+      </c>
+      <c r="C75" s="1">
+        <v>8.4218546999999998E-7</v>
+      </c>
+      <c r="D75" s="1">
+        <v>1.4201359E-6</v>
+      </c>
+      <c r="E75" s="1">
+        <v>9.06235581E-7</v>
+      </c>
+      <c r="F75" s="1">
+        <v>6.8424953799999997E-7</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A76">
+        <v>80</v>
+      </c>
+      <c r="C76" s="1">
+        <v>7.0157294299999998E-7</v>
+      </c>
+      <c r="D76" s="1">
+        <v>1.4925217299999999E-6</v>
+      </c>
+      <c r="E76" s="1">
+        <v>2.9146453299999999E-6</v>
+      </c>
+      <c r="F76" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A77">
+        <v>76</v>
+      </c>
+      <c r="C77" s="1">
+        <v>6.3524222400000004E-7</v>
+      </c>
+      <c r="D77" s="1">
+        <v>1.67644174E-6</v>
+      </c>
+      <c r="E77" s="1">
+        <v>1.69442526E-6</v>
+      </c>
+      <c r="F77" s="1">
+        <v>7.6195437300000005E-7</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A78">
+        <v>36</v>
+      </c>
+      <c r="B78" t="s">
+        <v>133</v>
+      </c>
+      <c r="C78" s="1">
+        <v>5.9877813399999997E-7</v>
+      </c>
+      <c r="D78" s="1">
+        <v>2.81258186E-7</v>
+      </c>
+      <c r="E78" s="1">
+        <v>1.6239798100000001E-6</v>
+      </c>
+      <c r="F78" s="1">
+        <v>6.1961397400000004E-7</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A79">
+        <v>64</v>
+      </c>
+      <c r="C79" s="1">
+        <v>3.9895428299999998E-7</v>
+      </c>
+      <c r="D79" s="1">
+        <v>0</v>
+      </c>
+      <c r="E79" s="1">
+        <v>3.8598514299999999E-7</v>
+      </c>
+      <c r="F79" s="1">
+        <v>8.04643697E-7</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A80">
+        <v>127</v>
+      </c>
+      <c r="C80" s="1">
+        <v>3.27280029E-7</v>
+      </c>
+      <c r="D80" s="1">
+        <v>0</v>
+      </c>
+      <c r="E80" s="1">
+        <v>0</v>
+      </c>
+      <c r="F80" s="1">
+        <v>5.1459721499999997E-7</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A81">
+        <v>38</v>
+      </c>
+      <c r="B81" t="s">
+        <v>135</v>
+      </c>
+      <c r="C81" s="1">
+        <v>3.1442008699999998E-7</v>
+      </c>
+      <c r="D81" s="1">
+        <v>1.72688921E-7</v>
+      </c>
+      <c r="E81" s="1">
+        <v>9.0899634999999999E-7</v>
+      </c>
+      <c r="F81" s="1">
+        <v>7.1190913900000003E-7</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A82">
+        <v>66</v>
+      </c>
+      <c r="C82" s="1">
+        <v>2.8442964299999999E-7</v>
+      </c>
+      <c r="D82" s="1">
+        <v>1.2213968900000001E-5</v>
+      </c>
+      <c r="E82" s="1">
+        <v>0</v>
+      </c>
+      <c r="F82" s="1">
+        <v>5.5913910199999997E-5</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A83">
+        <v>98</v>
+      </c>
+      <c r="C83" s="1">
+        <v>2.5740989700000002E-7</v>
+      </c>
+      <c r="D83" s="1">
+        <v>0</v>
+      </c>
+      <c r="E83" s="1">
+        <v>0</v>
+      </c>
+      <c r="F83" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A84">
+        <v>114</v>
+      </c>
+      <c r="C84" s="1">
+        <v>2.4931765599999998E-7</v>
+      </c>
+      <c r="D84" s="1">
+        <v>0</v>
+      </c>
+      <c r="E84" s="1">
+        <v>3.7227729200000001E-8</v>
+      </c>
+      <c r="F84" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A85">
+        <v>142</v>
+      </c>
+      <c r="C85" s="1">
+        <v>2.0010268100000001E-7</v>
+      </c>
+      <c r="D85" s="1">
+        <v>2.6695775999999998E-7</v>
+      </c>
+      <c r="E85" s="1">
+        <v>6.4361176499999995E-8</v>
+      </c>
+      <c r="F85" s="1">
+        <v>2.5440117499999998E-7</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A86">
+        <v>115</v>
+      </c>
+      <c r="C86" s="1">
+        <v>1.8899270300000001E-7</v>
+      </c>
+      <c r="D86" s="1">
+        <v>3.6709077000000003E-8</v>
+      </c>
+      <c r="E86" s="1">
+        <v>8.2803297700000001E-8</v>
+      </c>
+      <c r="F86" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A87">
+        <v>103</v>
+      </c>
+      <c r="C87" s="1">
+        <v>1.80330429E-7</v>
+      </c>
+      <c r="D87" s="1">
+        <v>0</v>
+      </c>
+      <c r="E87" s="1">
+        <v>0</v>
+      </c>
+      <c r="F87" s="1">
+        <v>1.2050695700000001E-7</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A88">
+        <v>131</v>
+      </c>
+      <c r="C88" s="1">
+        <v>1.79803354E-7</v>
+      </c>
+      <c r="D88" s="1">
+        <v>3.57218201E-9</v>
+      </c>
+      <c r="E88" s="1">
+        <v>0</v>
+      </c>
+      <c r="F88" s="1">
+        <v>1.10908168E-7</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A89">
+        <v>123</v>
+      </c>
+      <c r="C89" s="1">
+        <v>1.7521297799999999E-7</v>
+      </c>
+      <c r="D89" s="1">
+        <v>2.73034685E-7</v>
+      </c>
+      <c r="E89" s="1">
+        <v>2.8477415400000001E-7</v>
+      </c>
+      <c r="F89" s="1">
+        <v>3.6872126199999998E-8</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A90">
+        <v>152</v>
+      </c>
+      <c r="C90" s="1">
+        <v>1.69868599E-7</v>
+      </c>
+      <c r="D90" s="1">
+        <v>1.88053089E-7</v>
+      </c>
+      <c r="E90" s="1">
+        <v>2.2690991399999999E-7</v>
+      </c>
+      <c r="F90" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A91">
+        <v>112</v>
+      </c>
+      <c r="C91" s="1">
+        <v>1.6830096199999999E-7</v>
+      </c>
+      <c r="D91" s="1">
+        <v>5.4065771299999997E-8</v>
+      </c>
+      <c r="E91" s="1">
+        <v>4.4318747599999999E-7</v>
+      </c>
+      <c r="F91" s="1">
+        <v>1.90877445E-7</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A92">
+        <v>147</v>
+      </c>
+      <c r="C92" s="1">
+        <v>1.4852895300000001E-7</v>
+      </c>
+      <c r="D92" s="1">
+        <v>0</v>
+      </c>
+      <c r="E92" s="1">
+        <v>0</v>
+      </c>
+      <c r="F92" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A93">
+        <v>148</v>
+      </c>
+      <c r="C93" s="1">
+        <v>1.4624105799999999E-7</v>
+      </c>
+      <c r="D93" s="1">
+        <v>1.8097594299999999E-8</v>
+      </c>
+      <c r="E93" s="1">
+        <v>4.6371772900000002E-8</v>
+      </c>
+      <c r="F93" s="1">
+        <v>2.2117292599999999E-7</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A94">
+        <v>146</v>
+      </c>
+      <c r="C94" s="1">
+        <v>1.4550497E-7</v>
+      </c>
+      <c r="D94" s="1">
+        <v>0</v>
+      </c>
+      <c r="E94" s="1">
+        <v>1.2978749200000001E-7</v>
+      </c>
+      <c r="F94" s="1">
+        <v>9.1221071900000001E-9</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A95">
+        <v>132</v>
+      </c>
+      <c r="C95" s="1">
+        <v>1.27995144E-7</v>
+      </c>
+      <c r="D95" s="1">
+        <v>0</v>
+      </c>
+      <c r="E95" s="1">
+        <v>0</v>
+      </c>
+      <c r="F95" s="1">
+        <v>6.9430219199999997E-8</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A96">
+        <v>74</v>
+      </c>
+      <c r="C96" s="1">
+        <v>1.1672201500000001E-7</v>
+      </c>
+      <c r="D96" s="1">
+        <v>2.8329748000000002E-7</v>
+      </c>
+      <c r="E96" s="1">
+        <v>4.7053993799999997E-6</v>
+      </c>
+      <c r="F96" s="1">
+        <v>1.00998254E-7</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A97">
+        <v>104</v>
+      </c>
+      <c r="C97" s="1">
+        <v>1.15481686E-7</v>
+      </c>
+      <c r="D97" s="1">
+        <v>0</v>
+      </c>
+      <c r="E97" s="1">
+        <v>3.1028060799999998E-8</v>
+      </c>
+      <c r="F97" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A98">
+        <v>62</v>
+      </c>
+      <c r="C98" s="1">
+        <v>1.14900735E-7</v>
+      </c>
+      <c r="D98" s="1">
+        <v>0</v>
+      </c>
+      <c r="E98" s="1">
+        <v>9.32450762E-8</v>
+      </c>
+      <c r="F98" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A99">
+        <v>106</v>
+      </c>
+      <c r="C99" s="1">
+        <v>1.13293167E-7</v>
+      </c>
+      <c r="D99" s="1">
+        <v>0</v>
+      </c>
+      <c r="E99" s="1">
+        <v>0</v>
+      </c>
+      <c r="F99" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A100">
+        <v>116</v>
+      </c>
+      <c r="C100" s="1">
+        <v>1.0193632099999999E-7</v>
+      </c>
+      <c r="D100" s="1">
+        <v>0</v>
+      </c>
+      <c r="E100" s="1">
+        <v>0</v>
+      </c>
+      <c r="F100" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A101">
+        <v>125</v>
+      </c>
+      <c r="C101" s="1">
+        <v>9.6585494699999998E-8</v>
+      </c>
+      <c r="D101" s="1">
+        <v>3.1180054300000001E-8</v>
+      </c>
+      <c r="E101" s="1">
+        <v>3.3927155899999998E-8</v>
+      </c>
+      <c r="F101" s="1">
+        <v>1.1809878799999999E-9</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A102">
+        <v>113</v>
+      </c>
+      <c r="C102" s="1">
+        <v>8.9792565299999998E-8</v>
+      </c>
+      <c r="D102" s="1">
+        <v>0</v>
+      </c>
+      <c r="E102" s="1">
+        <v>1.4525772999999999E-8</v>
+      </c>
+      <c r="F102" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A103">
+        <v>129</v>
+      </c>
+      <c r="C103" s="1">
+        <v>8.6871075999999995E-8</v>
+      </c>
+      <c r="D103" s="1">
+        <v>3.8702762899999998E-9</v>
+      </c>
+      <c r="E103" s="1">
+        <v>1.17720562E-7</v>
+      </c>
+      <c r="F103" s="1">
+        <v>3.4242271E-8</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A104">
+        <v>87</v>
+      </c>
+      <c r="C104" s="1">
+        <v>8.4309230399999998E-8</v>
+      </c>
+      <c r="D104" s="1">
+        <v>6.5268662699999997E-8</v>
+      </c>
+      <c r="E104" s="1">
+        <v>4.0859182000000001E-8</v>
+      </c>
+      <c r="F104" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A105">
+        <v>135</v>
+      </c>
+      <c r="C105" s="1">
+        <v>8.0701788699999994E-8</v>
+      </c>
+      <c r="D105" s="1">
+        <v>0</v>
+      </c>
+      <c r="E105" s="1">
+        <v>3.75822834E-8</v>
+      </c>
+      <c r="F105" s="1">
+        <v>8.40715483E-8</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A106">
+        <v>141</v>
+      </c>
+      <c r="C106" s="1">
+        <v>6.4005228000000003E-8</v>
+      </c>
+      <c r="D106" s="1">
+        <v>0</v>
+      </c>
+      <c r="E106" s="1">
+        <v>0</v>
+      </c>
+      <c r="F106" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A107">
+        <v>118</v>
+      </c>
+      <c r="C107" s="1">
+        <v>6.1469512900000006E-8</v>
+      </c>
+      <c r="D107" s="1">
+        <v>0</v>
+      </c>
+      <c r="E107" s="1">
+        <v>2.4333168000000001E-8</v>
+      </c>
+      <c r="F107" s="1">
+        <v>4.6537761700000001E-8</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A108">
+        <v>58</v>
+      </c>
+      <c r="C108" s="1">
+        <v>5.9471588399999999E-8</v>
+      </c>
+      <c r="D108" s="1">
+        <v>0</v>
+      </c>
+      <c r="E108" s="1">
+        <v>0</v>
+      </c>
+      <c r="F108" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A109">
+        <v>83</v>
+      </c>
+      <c r="C109" s="1">
+        <v>5.6356191700000002E-8</v>
+      </c>
+      <c r="D109" s="1">
+        <v>1.0289393600000001E-6</v>
+      </c>
+      <c r="E109" s="1">
+        <v>5.1937783999999997E-6</v>
+      </c>
+      <c r="F109" s="1">
+        <v>1.1979420500000001E-6</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A110">
+        <v>63</v>
+      </c>
+      <c r="C110" s="1">
+        <v>3.5759662099999997E-8</v>
+      </c>
+      <c r="D110" s="1">
+        <v>7.2321343799999996E-10</v>
+      </c>
+      <c r="E110" s="1">
+        <v>1.28513881E-7</v>
+      </c>
+      <c r="F110" s="1">
+        <v>3.9661444099999998E-8</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A111">
+        <v>120</v>
+      </c>
+      <c r="C111" s="1">
+        <v>3.14286215E-8</v>
+      </c>
+      <c r="D111" s="1">
+        <v>0</v>
+      </c>
+      <c r="E111" s="1">
+        <v>0</v>
+      </c>
+      <c r="F111" s="1">
+        <v>3.3853405600000002E-8</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A112">
+        <v>99</v>
+      </c>
+      <c r="C112" s="1">
+        <v>2.6814387399999999E-8</v>
+      </c>
+      <c r="D112" s="1">
+        <v>0</v>
+      </c>
+      <c r="E112" s="1">
+        <v>0</v>
+      </c>
+      <c r="F112" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A113">
+        <v>72</v>
+      </c>
+      <c r="C113" s="1">
+        <v>1.8652610700000002E-8</v>
+      </c>
+      <c r="D113" s="1">
+        <v>2.0678824100000001E-7</v>
+      </c>
+      <c r="E113" s="1">
+        <v>1.16276733E-7</v>
+      </c>
+      <c r="F113" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A114">
+        <v>77</v>
+      </c>
+      <c r="C114" s="1">
+        <v>1.33462838E-8</v>
+      </c>
+      <c r="D114" s="1">
+        <v>0</v>
+      </c>
+      <c r="E114" s="1">
+        <v>0</v>
+      </c>
+      <c r="F114" s="1">
+        <v>6.0773549199999999E-9</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A115">
+        <v>78</v>
+      </c>
+      <c r="C115" s="1">
+        <v>8.3785215999999996E-10</v>
+      </c>
+      <c r="D115" s="1">
+        <v>6.1128530199999997E-8</v>
+      </c>
+      <c r="E115" s="1">
+        <v>1.51728724E-7</v>
+      </c>
+      <c r="F115" s="1">
+        <v>6.3304836E-7</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A116">
+        <v>56</v>
+      </c>
+      <c r="C116" s="1">
+        <v>0</v>
+      </c>
+      <c r="D116" s="1">
+        <v>4.1345753199999999E-8</v>
+      </c>
+      <c r="E116" s="1">
+        <v>1.2396069999999999E-6</v>
+      </c>
+      <c r="F116" s="1">
+        <v>2.4621507500000002E-6</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A117">
+        <v>67</v>
+      </c>
+      <c r="C117" s="1">
+        <v>0</v>
+      </c>
+      <c r="D117" s="1">
+        <v>4.6061450999999999E-7</v>
+      </c>
+      <c r="E117" s="1">
+        <v>0</v>
+      </c>
+      <c r="F117" s="1">
+        <v>1.8097601E-7</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A118">
+        <v>71</v>
+      </c>
+      <c r="C118" s="1">
+        <v>0</v>
+      </c>
+      <c r="D118" s="1">
+        <v>0</v>
+      </c>
+      <c r="E118" s="1">
+        <v>5.5863658900000001E-6</v>
+      </c>
+      <c r="F118" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A119">
+        <v>73</v>
+      </c>
+      <c r="C119" s="1">
+        <v>0</v>
+      </c>
+      <c r="D119" s="1">
+        <v>9.2423999099999999E-8</v>
+      </c>
+      <c r="E119" s="1">
+        <v>1.57659396E-7</v>
+      </c>
+      <c r="F119" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A120">
+        <v>75</v>
+      </c>
+      <c r="C120" s="1">
+        <v>0</v>
+      </c>
+      <c r="D120" s="1">
+        <v>1.1964458499999999E-7</v>
+      </c>
+      <c r="E120" s="1">
+        <v>0</v>
+      </c>
+      <c r="F120" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A121">
+        <v>79</v>
+      </c>
+      <c r="C121" s="1">
+        <v>0</v>
+      </c>
+      <c r="D121" s="1">
+        <v>9.1944744199999995E-8</v>
+      </c>
+      <c r="E121" s="1">
+        <v>0</v>
+      </c>
+      <c r="F121" s="1">
+        <v>2.3969073400000001E-7</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A122">
+        <v>86</v>
+      </c>
+      <c r="C122" s="1">
+        <v>0</v>
+      </c>
+      <c r="D122" s="1">
+        <v>1.3725822E-6</v>
+      </c>
+      <c r="E122" s="1">
+        <v>1.38080029E-6</v>
+      </c>
+      <c r="F122" s="1">
+        <v>3.0642258500000002E-7</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A123">
+        <v>93</v>
+      </c>
+      <c r="C123" s="1">
+        <v>0</v>
+      </c>
+      <c r="D123" s="1">
+        <v>0</v>
+      </c>
+      <c r="E123" s="1">
+        <v>0</v>
+      </c>
+      <c r="F123" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A124">
+        <v>94</v>
+      </c>
+      <c r="C124" s="1">
+        <v>0</v>
+      </c>
+      <c r="D124" s="1">
+        <v>1.7758931599999998E-8</v>
+      </c>
+      <c r="E124" s="1">
+        <v>0</v>
+      </c>
+      <c r="F124" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A125">
+        <v>95</v>
+      </c>
+      <c r="C125" s="1">
+        <v>0</v>
+      </c>
+      <c r="D125" s="1">
+        <v>0</v>
+      </c>
+      <c r="E125" s="1">
+        <v>0</v>
+      </c>
+      <c r="F125" s="1">
+        <v>1.3591400800000001E-7</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A126">
+        <v>96</v>
+      </c>
+      <c r="C126" s="1">
+        <v>0</v>
+      </c>
+      <c r="D126" s="1">
+        <v>8.4516424500000005E-8</v>
+      </c>
+      <c r="E126" s="1">
+        <v>8.3119505900000005E-8</v>
+      </c>
+      <c r="F126" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A127">
+        <v>97</v>
+      </c>
+      <c r="C127" s="1">
+        <v>0</v>
+      </c>
+      <c r="D127" s="1">
+        <v>0</v>
+      </c>
+      <c r="E127" s="1">
+        <v>0</v>
+      </c>
+      <c r="F127" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A128">
+        <v>100</v>
+      </c>
+      <c r="C128" s="1">
+        <v>0</v>
+      </c>
+      <c r="D128" s="1">
+        <v>3.9353158200000003E-8</v>
+      </c>
+      <c r="E128" s="1">
+        <v>1.4038643E-7</v>
+      </c>
+      <c r="F128" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="129" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A129">
+        <v>101</v>
+      </c>
+      <c r="C129" s="1">
+        <v>0</v>
+      </c>
+      <c r="D129" s="1">
+        <v>5.6964270300000002E-7</v>
+      </c>
+      <c r="E129" s="1">
+        <v>0</v>
+      </c>
+      <c r="F129" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="130" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A130">
+        <v>102</v>
+      </c>
+      <c r="C130" s="1">
+        <v>0</v>
+      </c>
+      <c r="D130" s="1">
+        <v>0</v>
+      </c>
+      <c r="E130" s="1">
+        <v>6.5297419899999999E-8</v>
+      </c>
+      <c r="F130" s="1">
+        <v>6.0190751100000004E-8</v>
+      </c>
+    </row>
+    <row r="131" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A131">
+        <v>105</v>
+      </c>
+      <c r="C131" s="1">
+        <v>0</v>
+      </c>
+      <c r="D131" s="1">
+        <v>1.0694196399999999E-7</v>
+      </c>
+      <c r="E131" s="1">
+        <v>8.8326065000000007E-9</v>
+      </c>
+      <c r="F131" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="132" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A132">
+        <v>107</v>
+      </c>
+      <c r="C132" s="1">
+        <v>0</v>
+      </c>
+      <c r="D132" s="1">
+        <v>0</v>
+      </c>
+      <c r="E132" s="1">
+        <v>0</v>
+      </c>
+      <c r="F132" s="1">
+        <v>1.08064059E-7</v>
+      </c>
+    </row>
+    <row r="133" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A133">
+        <v>109</v>
+      </c>
+      <c r="C133" s="1">
+        <v>0</v>
+      </c>
+      <c r="D133" s="1">
+        <v>5.4482506500000002E-8</v>
+      </c>
+      <c r="E133" s="1">
+        <v>0</v>
+      </c>
+      <c r="F133" s="1">
+        <v>1.2754973E-7</v>
+      </c>
+    </row>
+    <row r="134" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A134">
+        <v>110</v>
+      </c>
+      <c r="C134" s="1">
+        <v>0</v>
+      </c>
+      <c r="D134" s="1">
+        <v>0</v>
+      </c>
+      <c r="E134" s="1">
+        <v>0</v>
+      </c>
+      <c r="F134" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="135" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A135">
+        <v>111</v>
+      </c>
+      <c r="C135" s="1">
+        <v>0</v>
+      </c>
+      <c r="D135" s="1">
+        <v>8.7846013799999999E-8</v>
+      </c>
+      <c r="E135" s="1">
+        <v>0</v>
+      </c>
+      <c r="F135" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="136" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A136">
+        <v>117</v>
+      </c>
+      <c r="C136" s="1">
+        <v>0</v>
+      </c>
+      <c r="D136" s="1">
+        <v>1.64237646E-7</v>
+      </c>
+      <c r="E136" s="1">
+        <v>0</v>
+      </c>
+      <c r="F136" s="1">
+        <v>4.1530104900000001E-7</v>
+      </c>
+    </row>
+    <row r="137" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A137">
+        <v>119</v>
+      </c>
+      <c r="C137" s="1">
+        <v>0</v>
+      </c>
+      <c r="D137" s="1">
+        <v>7.4826063400000003E-7</v>
+      </c>
+      <c r="E137" s="1">
+        <v>0</v>
+      </c>
+      <c r="F137" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="138" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A138">
+        <v>121</v>
+      </c>
+      <c r="C138" s="1">
+        <v>0</v>
+      </c>
+      <c r="D138" s="1">
+        <v>0</v>
+      </c>
+      <c r="E138" s="1">
+        <v>2.2815219799999999E-7</v>
+      </c>
+      <c r="F138" s="1">
+        <v>1.62913051E-8</v>
+      </c>
+    </row>
+    <row r="139" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A139">
+        <v>122</v>
+      </c>
+      <c r="C139" s="1">
+        <v>0</v>
+      </c>
+      <c r="D139" s="1">
+        <v>2.7196466499999999E-7</v>
+      </c>
+      <c r="E139" s="1">
+        <v>0</v>
+      </c>
+      <c r="F139" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="140" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A140">
+        <v>124</v>
+      </c>
+      <c r="C140" s="1">
+        <v>0</v>
+      </c>
+      <c r="D140" s="1">
+        <v>0</v>
+      </c>
+      <c r="E140" s="1">
+        <v>0</v>
+      </c>
+      <c r="F140" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="141" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A141">
+        <v>126</v>
+      </c>
+      <c r="C141" s="1">
+        <v>0</v>
+      </c>
+      <c r="D141" s="1">
+        <v>0</v>
+      </c>
+      <c r="E141" s="1">
+        <v>1.05612378E-7</v>
+      </c>
+      <c r="F141" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="142" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A142">
+        <v>128</v>
+      </c>
+      <c r="C142" s="1">
+        <v>0</v>
+      </c>
+      <c r="D142" s="1">
+        <v>2.2047137100000001E-7</v>
+      </c>
+      <c r="E142" s="1">
+        <v>0</v>
+      </c>
+      <c r="F142" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="143" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A143">
+        <v>130</v>
+      </c>
+      <c r="C143" s="1">
+        <v>0</v>
+      </c>
+      <c r="D143" s="1">
+        <v>0</v>
+      </c>
+      <c r="E143" s="1">
+        <v>2.2049008000000001E-7</v>
+      </c>
+      <c r="F143" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="144" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A144">
+        <v>133</v>
+      </c>
+      <c r="C144" s="1">
+        <v>0</v>
+      </c>
+      <c r="D144" s="1">
+        <v>0</v>
+      </c>
+      <c r="E144" s="1">
+        <v>0</v>
+      </c>
+      <c r="F144" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="145" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A145">
+        <v>134</v>
+      </c>
+      <c r="C145" s="1">
+        <v>0</v>
+      </c>
+      <c r="D145" s="1">
+        <v>0</v>
+      </c>
+      <c r="E145" s="1">
+        <v>0</v>
+      </c>
+      <c r="F145" s="1">
+        <v>1.2153304799999999E-8</v>
+      </c>
+    </row>
+    <row r="146" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A146">
+        <v>136</v>
+      </c>
+      <c r="C146" s="1">
+        <v>0</v>
+      </c>
+      <c r="D146" s="1">
+        <v>0</v>
+      </c>
+      <c r="E146" s="1">
+        <v>2.7078429899999999E-8</v>
+      </c>
+      <c r="F146" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="147" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A147">
+        <v>137</v>
+      </c>
+      <c r="C147" s="1">
+        <v>0</v>
+      </c>
+      <c r="D147" s="1">
+        <v>0</v>
+      </c>
+      <c r="E147" s="1">
+        <v>0</v>
+      </c>
+      <c r="F147" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="148" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A148">
+        <v>138</v>
+      </c>
+      <c r="C148" s="1">
+        <v>0</v>
+      </c>
+      <c r="D148" s="1">
+        <v>0</v>
+      </c>
+      <c r="E148" s="1">
+        <v>1.7311160399999999E-7</v>
+      </c>
+      <c r="F148" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="149" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A149">
+        <v>139</v>
+      </c>
+      <c r="C149" s="1">
+        <v>0</v>
+      </c>
+      <c r="D149" s="1">
+        <v>0</v>
+      </c>
+      <c r="E149" s="1">
+        <v>5.3095732000000002E-8</v>
+      </c>
+      <c r="F149" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="150" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A150">
+        <v>140</v>
+      </c>
+      <c r="C150" s="1">
+        <v>0</v>
+      </c>
+      <c r="D150" s="1">
+        <v>1.87695076E-7</v>
+      </c>
+      <c r="E150" s="1">
+        <v>0</v>
+      </c>
+      <c r="F150" s="1">
+        <v>1.2056208300000001E-8</v>
+      </c>
+    </row>
+    <row r="151" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A151">
+        <v>143</v>
+      </c>
+      <c r="C151" s="1">
+        <v>0</v>
+      </c>
+      <c r="D151" s="1">
+        <v>2.8386867900000001E-8</v>
+      </c>
+      <c r="E151" s="1">
+        <v>0</v>
+      </c>
+      <c r="F151" s="1">
+        <v>1.6529748499999999E-7</v>
+      </c>
+    </row>
+    <row r="152" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A152">
+        <v>144</v>
+      </c>
+      <c r="C152" s="1">
+        <v>0</v>
+      </c>
+      <c r="D152" s="1">
+        <v>0</v>
+      </c>
+      <c r="E152" s="1">
+        <v>3.9111095499999998E-7</v>
+      </c>
+      <c r="F152" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="153" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A153">
+        <v>145</v>
+      </c>
+      <c r="C153" s="1">
+        <v>0</v>
+      </c>
+      <c r="D153" s="1">
+        <v>0</v>
+      </c>
+      <c r="E153" s="1">
+        <v>0</v>
+      </c>
+      <c r="F153" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="154" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A154">
+        <v>149</v>
+      </c>
+      <c r="C154" s="1">
+        <v>0</v>
+      </c>
+      <c r="D154" s="1">
+        <v>1.9932128700000002E-9</v>
+      </c>
+      <c r="E154" s="1">
+        <v>0</v>
+      </c>
+      <c r="F154" s="1">
+        <v>6.43119364E-8</v>
+      </c>
+    </row>
+    <row r="155" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A155">
+        <v>150</v>
+      </c>
+      <c r="C155" s="1">
+        <v>0</v>
+      </c>
+      <c r="D155" s="1">
+        <v>0</v>
+      </c>
+      <c r="E155" s="1">
+        <v>0</v>
+      </c>
+      <c r="F155" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="156" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A156">
+        <v>151</v>
+      </c>
+      <c r="C156" s="1">
+        <v>0</v>
+      </c>
+      <c r="D156" s="1">
+        <v>8.0558488599999999E-9</v>
+      </c>
+      <c r="E156" s="1">
+        <v>1.7105500699999999E-7</v>
+      </c>
+      <c r="F156" s="1">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState ref="A4:F156">
+    <sortCondition descending="1" ref="C9"/>
+  </sortState>
+  <conditionalFormatting sqref="C4:C156">
+    <cfRule type="dataBar" priority="4">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF638EC6"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{AC2358C7-8F99-4FA4-B63B-511F158B40EA}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D4:D156">
+    <cfRule type="dataBar" priority="3">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF638EC6"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{DE29EE2F-3AFD-487C-B509-99A897B0171A}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E4:E156">
+    <cfRule type="dataBar" priority="2">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF638EC6"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{CA97CA59-F0CB-4182-A425-7F1F0F590237}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F4:F156">
+    <cfRule type="dataBar" priority="1">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF638EC6"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{76135D19-5DA4-4129-A931-1C2535976D18}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
+      <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{AC2358C7-8F99-4FA4-B63B-511F158B40EA}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FF638EC6"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>C4:C156</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{DE29EE2F-3AFD-487C-B509-99A897B0171A}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FF638EC6"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>D4:D156</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{CA97CA59-F0CB-4182-A425-7F1F0F590237}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FF638EC6"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>E4:E156</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{76135D19-5DA4-4129-A931-1C2535976D18}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FF638EC6"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>F4:F156</xm:sqref>
+        </x14:conditionalFormatting>
+      </x14:conditionalFormattings>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>